<commit_message>
Completed long term outlook view.
</commit_message>
<xml_diff>
--- a/src/assets/years/2023.xlsx
+++ b/src/assets/years/2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD89ED0-D429-4F54-8925-409E2A969D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF015E7-863D-4EF0-AE58-B86D8EA0063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3285" windowWidth="29040" windowHeight="15840" xr2:uid="{998BE1DA-C037-4508-8C33-93B2F93493F5}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="113">
   <si>
     <t>indicator</t>
   </si>
@@ -453,6 +453,15 @@
   </si>
   <si>
     <t>Marge de manoeuvre permettant d'accroître les dépenses ou de réduire les impôts tout en assurant la viabilité financière.</t>
+  </si>
+  <si>
+    <t>fsr_intro</t>
+  </si>
+  <si>
+    <t>The OPBO has prepared fact sheets for the provinces and territories.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+  </si>
+  <si>
+    <t>Le BDPB a préparé des fiches d'information pour les provinces et les territoires.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
   </si>
 </sst>
 </file>
@@ -872,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7255F49-EEAA-44D0-BDAF-26A02A9AE815}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,179 +922,186 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>96</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
@@ -1146,6 +1162,10 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added simple references to the published report.
</commit_message>
<xml_diff>
--- a/src/assets/years/2023.xlsx
+++ b/src/assets/years/2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\VanheR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF015E7-863D-4EF0-AE58-B86D8EA0063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7CD317-2F79-4EAE-B3D1-37E3038E7524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3285" windowWidth="29040" windowHeight="15840" xr2:uid="{998BE1DA-C037-4508-8C33-93B2F93493F5}"/>
   </bookViews>
@@ -42,10 +42,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={3F29968F-C5CE-440C-94C6-7125F04DC27E}</author>
+    <author>tc={5EBFEEF0-71CA-4E4D-8875-9DF48418AE8B}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{3F29968F-C5CE-440C-94C6-7125F04DC27E}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5EBFEEF0-71CA-4E4D-8875-9DF48418AE8B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="114">
   <si>
     <t>indicator</t>
   </si>
@@ -311,10 +311,40 @@
     <t xml:space="preserve">Because provincial-local government spending is growing more slowly in provinces than in the Territories in our projection, the Territorial Formula Financing does not keep pace with territorial program spending. We therefore project revenue declines (as a share of the economy) under the current formula. </t>
   </si>
   <si>
+    <t>Value (or en)</t>
+  </si>
+  <si>
+    <t>(fr)</t>
+  </si>
+  <si>
+    <t>fsr_poster_url</t>
+  </si>
+  <si>
+    <t>https://distribution-i696d61676573.pbo-dpb.ca/17394f7f5b7d2cd2405e3a05d1082eb72400241c249bb030a32cabf60b3ac77e</t>
+  </si>
+  <si>
+    <t>https://distribution-i696d61676573.pbo-dpb.ca/f5a6d162ca59b837a46677d33f93a808d448d23ce2f3d0f728a1b7615ca4c325</t>
+  </si>
+  <si>
+    <t>fsr_url</t>
+  </si>
+  <si>
+    <t>fsr_intro</t>
+  </si>
+  <si>
+    <t>The OPBO has prepared fact sheets for the provinces and territories.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+  </si>
+  <si>
+    <t>Le BDPB a préparé des fiches d'information pour les provinces et les territoires.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+  </si>
+  <si>
     <t>infographic_subsus_tl</t>
   </si>
   <si>
     <t>Current fiscal policy in Quebec, Saskatchewa, Nova Scotia, New Brunswich and Alberta is **sustainable**.</t>
+  </si>
+  <si>
+    <t>La politique financière actuelle au Québec, en Saskatchewan, en Nouvelle-Écosse, au Nouveau-Brunswick et en Alberta est **viable**.</t>
   </si>
   <si>
     <t>infographic_subsus_tr</t>
@@ -323,28 +353,16 @@
     <t>Fiscal policy in remaining provinces and territories is **not sustainable**.</t>
   </si>
   <si>
+    <t>La politique financière des autres provinces et territoires n'est **pas viable**.</t>
+  </si>
+  <si>
     <t>infographic_subsus_br</t>
   </si>
   <si>
     <t>**Biggest contributors** to the positive subnational fiscal gap are British Columbia, Manitoba, and Ontario.</t>
   </si>
   <si>
-    <t>infographic_subsus_legend_fg_range_sunny</t>
-  </si>
-  <si>
-    <t>infographic_subsus_legend_fg_range_cloudy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -1.8 to -0.1</t>
-  </si>
-  <si>
-    <t>-1,8 à -0,1</t>
-  </si>
-  <si>
-    <t>0.2 to 6.4</t>
-  </si>
-  <si>
-    <t>0,2 à 6,4</t>
+    <t>La Colombie-Britannique, le Manitoba et l'Ontario sont **les principaux responsables** de l'écart financier positif des administrations infranationales.</t>
   </si>
   <si>
     <t>infographic_subsus_legend_fg_title</t>
@@ -356,25 +374,22 @@
     <t>Écart financier (% du PIB)</t>
   </si>
   <si>
-    <t>La politique financière des autres provinces et territoires n'est **pas viable**.</t>
+    <t>infographic_subsus_legend_fg_range_sunny</t>
   </si>
   <si>
-    <t>La politique financière actuelle au Québec, en Saskatchewan, en Nouvelle-Écosse, au Nouveau-Brunswick et en Alberta est **viable**.</t>
+    <t xml:space="preserve"> -1.8 to -0.1</t>
   </si>
   <si>
-    <t>Value (or en)</t>
+    <t>-1,8 à -0,1</t>
   </si>
   <si>
-    <t>(fr)</t>
+    <t>infographic_subsus_legend_fg_range_cloudy</t>
   </si>
   <si>
-    <t>fsr_url</t>
+    <t>0.2 to 6.4</t>
   </si>
   <si>
-    <t>Complex state needs further explanation</t>
-  </si>
-  <si>
-    <t>État complexe nécessite plus d'explications</t>
+    <t>0,2 à 6,4</t>
   </si>
   <si>
     <t>infographic_subsus_legend_fg_range_partly</t>
@@ -389,19 +404,16 @@
     <t>infographic_lt_perspective_fed_is_sustainable</t>
   </si>
   <si>
-    <t>infographic_lt_perspective_fed_legend</t>
+    <t>TRUE</t>
   </si>
   <si>
-    <t>TRUE</t>
+    <t>infographic_lt_perspective_fed_legend</t>
   </si>
   <si>
     <t>Current fiscal policy at the federal level **is sustainable** over the long term.</t>
   </si>
   <si>
     <t>La politique financière actuelle au niveau fédéral **est viable** à long terme.</t>
-  </si>
-  <si>
-    <t>La Colombie-Britannique, le Manitoba et l'Ontario sont **les principaux responsables** de l'écart financier positif des administrations infranationales.</t>
   </si>
   <si>
     <t>infographic_lt_perspective_ppp_is_sustainable</t>
@@ -428,10 +440,10 @@
     <t>La politique financière actuelle **est viable** à long terme.</t>
   </si>
   <si>
-    <t>Changes in **revenues or program spending** required to stabilize the government's **net debt-to-GDP ratio** over the long term.</t>
+    <t>infographic_fg_definition</t>
   </si>
   <si>
-    <t>infographic_fg_definition</t>
+    <t>Changes in **revenues or program spending** required to stabilize the government's **net debt-to-GDP ratio** over the long term.</t>
   </si>
   <si>
     <t>Changements à apporter aux **revenus ou aux dépenses** de programme pour stabiliser le **ratio de la dette nette du gouvernement au PIB**.</t>
@@ -443,32 +455,23 @@
     <t>Permanent changes in revenues or program spending required to stabilize debt-to-GDP ratio.</t>
   </si>
   <si>
+    <t>Modifications permanentes des prevenus ou des dépenses de programme nécessaires pour stabiliser le ratio de la dette au PIB.</t>
+  </si>
+  <si>
     <t>infographic_fg_neg_definition</t>
   </si>
   <si>
     <t>Room available to inscrease spending or reduce taxes while maintaining fiscal sustainability.</t>
   </si>
   <si>
-    <t>Modifications permanentes des prevenus ou des dépenses de programme nécessaires pour stabiliser le ratio de la dette au PIB.</t>
-  </si>
-  <si>
     <t>Marge de manoeuvre permettant d'accroître les dépenses ou de réduire les impôts tout en assurant la viabilité financière.</t>
-  </si>
-  <si>
-    <t>fsr_intro</t>
-  </si>
-  <si>
-    <t>The OPBO has prepared fact sheets for the provinces and territories.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
-  </si>
-  <si>
-    <t>Le BDPB a préparé des fiches d'information pour les provinces et les territoires.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +486,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -505,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -514,7 +523,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -838,7 +846,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A2" dT="2023-08-10T14:17:34.14" personId="{75396AFA-A819-4B8F-B56E-DD6CE5DE5E52}" id="{3F29968F-C5CE-440C-94C6-7125F04DC27E}">
+  <threadedComment ref="A2" dT="2023-08-10T14:17:34.14" personId="{75396AFA-A819-4B8F-B56E-DD6CE5DE5E52}" id="{5EBFEEF0-71CA-4E4D-8875-9DF48418AE8B}">
     <text>Future versions of this tool could allow users to navigate back in time and see previous year’s data with a slider, selector or a similar UI component.</text>
   </threadedComment>
 </ThreadedComments>
@@ -881,291 +889,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7255F49-EEAA-44D0-BDAF-26A02A9AE815}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="74.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>80</v>
+      <c r="B1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>2023</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>76</v>
+      <c r="C8" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="5" t="s">
         <v>86</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>96</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>108</v>
+      <c r="B19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="C20" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1178,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59BEA0E-1C9D-4B0B-A62B-B75C30F6159A}">
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="D1" s="1">
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="E1" s="1">
-        <v>2075</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1213,7 +1168,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D2">
         <v>0.6</v>
@@ -1229,15 +1184,6 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>31.4</v>
-      </c>
-      <c r="D3">
-        <v>38.6</v>
-      </c>
-      <c r="E3">
-        <v>43.8</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1247,7 +1193,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>1.5</v>
@@ -1264,10 +1210,10 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
         <v>0.6</v>
@@ -1332,7 +1278,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>27</v>
+        <v>26.9</v>
       </c>
       <c r="D9">
         <v>26.4</v>
@@ -1349,13 +1295,13 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>25.8</v>
+        <v>25.6</v>
       </c>
       <c r="D10">
         <v>25.9</v>
       </c>
       <c r="E10">
-        <v>25.9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1366,10 +1312,10 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1383,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D12">
         <v>0.9</v>
@@ -1400,13 +1346,13 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>20.3</v>
+        <v>19.2</v>
       </c>
       <c r="D13">
-        <v>13.7</v>
+        <v>13.6</v>
       </c>
       <c r="E13">
-        <v>13.3</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>1.3</v>
@@ -1433,15 +1379,6 @@
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15">
-        <v>24.2</v>
-      </c>
-      <c r="D15">
-        <v>31.4</v>
-      </c>
-      <c r="E15">
-        <v>37.6</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1451,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="D16">
         <v>2.1</v>
@@ -1468,7 +1405,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="D17">
         <v>1.1000000000000001</v>
@@ -1485,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D18">
         <v>1.1000000000000001</v>
@@ -1502,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="D19">
         <v>4.2</v>
@@ -1519,7 +1456,7 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="D20">
         <v>3.9</v>
@@ -1553,10 +1490,10 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>18.100000000000001</v>
+        <v>18.2</v>
       </c>
       <c r="D22">
-        <v>18.600000000000001</v>
+        <v>18.7</v>
       </c>
       <c r="E22">
         <v>19</v>
@@ -1570,13 +1507,13 @@
         <v>11</v>
       </c>
       <c r="C23">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0.4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1590,7 +1527,7 @@
         <v>0.7</v>
       </c>
       <c r="D24">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>-0.1</v>
@@ -1604,13 +1541,13 @@
         <v>13</v>
       </c>
       <c r="C25">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="D25">
-        <v>-4.5999999999999996</v>
+        <v>-5</v>
       </c>
       <c r="E25">
-        <v>-5.0999999999999996</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1621,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="C26">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D26">
         <v>0.6</v>
@@ -1637,15 +1574,6 @@
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27">
-        <v>33</v>
-      </c>
-      <c r="D27">
-        <v>41.2</v>
-      </c>
-      <c r="E27">
-        <v>47.4</v>
-      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1655,7 +1583,7 @@
         <v>4</v>
       </c>
       <c r="C28">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="D28">
         <v>0.9</v>
@@ -1672,7 +1600,7 @@
         <v>5</v>
       </c>
       <c r="C29">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="D29">
         <v>0.3</v>
@@ -1689,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D30">
         <v>0.7</v>
@@ -1706,7 +1634,7 @@
         <v>7</v>
       </c>
       <c r="C31">
-        <v>4.2</v>
+        <v>3.9</v>
       </c>
       <c r="D31">
         <v>2.9</v>
@@ -1723,7 +1651,7 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="D32">
         <v>3.9</v>
@@ -1740,13 +1668,13 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="D33">
-        <v>25.4</v>
+        <v>25.5</v>
       </c>
       <c r="E33">
-        <v>26.9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1757,7 +1685,7 @@
         <v>10</v>
       </c>
       <c r="C34">
-        <v>26.1</v>
+        <v>26.2</v>
       </c>
       <c r="D34">
         <v>27.1</v>
@@ -1774,13 +1702,13 @@
         <v>11</v>
       </c>
       <c r="C35">
-        <v>-0.8</v>
+        <v>-1</v>
       </c>
       <c r="D35">
-        <v>-1.7</v>
+        <v>-1.6</v>
       </c>
       <c r="E35">
-        <v>-0.6</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D36">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="E36">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1808,13 +1736,13 @@
         <v>13</v>
       </c>
       <c r="C37">
-        <v>7</v>
+        <v>10.4</v>
       </c>
       <c r="D37">
-        <v>60.8</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="E37">
-        <v>109.4</v>
+        <v>112.3</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,15 +1769,6 @@
       <c r="B39" t="s">
         <v>3</v>
       </c>
-      <c r="C39">
-        <v>27.6</v>
-      </c>
-      <c r="D39">
-        <v>31.8</v>
-      </c>
-      <c r="E39">
-        <v>37.200000000000003</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1859,7 +1778,7 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D40">
         <v>1.7</v>
@@ -1876,10 +1795,10 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D41">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E41">
         <v>0.6</v>
@@ -1893,7 +1812,7 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="D42">
         <v>1.2</v>
@@ -1910,13 +1829,13 @@
         <v>7</v>
       </c>
       <c r="C43">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D43">
         <v>3.7</v>
       </c>
       <c r="E43">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,7 +1846,7 @@
         <v>8</v>
       </c>
       <c r="C44">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -1944,13 +1863,13 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>31.3</v>
+        <v>30.9</v>
       </c>
       <c r="D45">
-        <v>29.4</v>
+        <v>29.3</v>
       </c>
       <c r="E45">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1961,10 +1880,10 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>31.1</v>
+        <v>30.5</v>
       </c>
       <c r="D46">
-        <v>31.4</v>
+        <v>31.5</v>
       </c>
       <c r="E46">
         <v>32.200000000000003</v>
@@ -1978,13 +1897,13 @@
         <v>11</v>
       </c>
       <c r="C47">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D47">
-        <v>-2</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="E47">
-        <v>-4</v>
+        <v>-4.2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,10 +1917,10 @@
         <v>2.6</v>
       </c>
       <c r="D48">
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="E48">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,13 +1931,13 @@
         <v>13</v>
       </c>
       <c r="C49">
-        <v>35</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="D49">
-        <v>78.900000000000006</v>
+        <v>84.6</v>
       </c>
       <c r="E49">
-        <v>167.9</v>
+        <v>177.1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2029,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="C50">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2045,15 +1964,6 @@
       <c r="B51" t="s">
         <v>3</v>
       </c>
-      <c r="C51">
-        <v>40.6</v>
-      </c>
-      <c r="D51">
-        <v>52</v>
-      </c>
-      <c r="E51">
-        <v>56.2</v>
-      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2063,7 +1973,7 @@
         <v>4</v>
       </c>
       <c r="C52">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>0.8</v>
@@ -2080,7 +1990,7 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D53">
         <v>-0.1</v>
@@ -2097,7 +2007,7 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>0.9</v>
@@ -2114,7 +2024,7 @@
         <v>7</v>
       </c>
       <c r="C55">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="D55">
         <v>2.8</v>
@@ -2131,7 +2041,7 @@
         <v>8</v>
       </c>
       <c r="C56">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="D56">
         <v>4.0999999999999996</v>
@@ -2148,13 +2058,13 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>32.799999999999997</v>
+        <v>32.9</v>
       </c>
       <c r="D57">
         <v>33.6</v>
       </c>
       <c r="E57">
-        <v>33.5</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2165,7 +2075,7 @@
         <v>10</v>
       </c>
       <c r="C58">
-        <v>30.9</v>
+        <v>31.1</v>
       </c>
       <c r="D58">
         <v>32.5</v>
@@ -2182,13 +2092,13 @@
         <v>11</v>
       </c>
       <c r="C59">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="D59">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E59">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2202,7 +2112,7 @@
         <v>1.9</v>
       </c>
       <c r="D60">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E60">
         <v>0.1</v>
@@ -2216,13 +2126,13 @@
         <v>13</v>
       </c>
       <c r="C61">
-        <v>19.399999999999999</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="D61">
-        <v>6.4</v>
+        <v>5.6</v>
       </c>
       <c r="E61">
-        <v>-4.5999999999999996</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2239,7 +2149,7 @@
         <v>-0.7</v>
       </c>
       <c r="E62">
-        <v>-0.4</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2249,15 +2159,6 @@
       <c r="B63" t="s">
         <v>3</v>
       </c>
-      <c r="C63">
-        <v>42.4</v>
-      </c>
-      <c r="D63">
-        <v>61.6</v>
-      </c>
-      <c r="E63">
-        <v>67.5</v>
-      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2267,13 +2168,13 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D64">
         <v>0.8</v>
       </c>
       <c r="E64">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2301,7 +2202,7 @@
         <v>6</v>
       </c>
       <c r="C66">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="D66">
         <v>1.6</v>
@@ -2324,7 +2225,7 @@
         <v>2.8</v>
       </c>
       <c r="E67">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2335,7 +2236,7 @@
         <v>8</v>
       </c>
       <c r="C68">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
       <c r="D68">
         <v>4.2</v>
@@ -2352,7 +2253,7 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>24.1</v>
+        <v>24</v>
       </c>
       <c r="D69">
         <v>23.8</v>
@@ -2369,10 +2270,10 @@
         <v>10</v>
       </c>
       <c r="C70">
-        <v>23.4</v>
+        <v>22.2</v>
       </c>
       <c r="D70">
-        <v>23.8</v>
+        <v>23.9</v>
       </c>
       <c r="E70">
         <v>24.1</v>
@@ -2386,13 +2287,13 @@
         <v>11</v>
       </c>
       <c r="C71">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="E71">
-        <v>-0.5</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2403,13 +2304,13 @@
         <v>12</v>
       </c>
       <c r="C72">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D72">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E72">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2420,13 +2321,13 @@
         <v>13</v>
       </c>
       <c r="C73">
-        <v>30.5</v>
+        <v>30.4</v>
       </c>
       <c r="D73">
-        <v>41.1</v>
+        <v>43.6</v>
       </c>
       <c r="E73">
-        <v>75.599999999999994</v>
+        <v>78.8</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,7 +2338,7 @@
         <v>2</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -2453,15 +2354,6 @@
       <c r="B75" t="s">
         <v>3</v>
       </c>
-      <c r="C75">
-        <v>38.5</v>
-      </c>
-      <c r="D75">
-        <v>48.1</v>
-      </c>
-      <c r="E75">
-        <v>55.2</v>
-      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -2471,7 +2363,7 @@
         <v>4</v>
       </c>
       <c r="C76">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="D76">
         <v>0.7</v>
@@ -2488,7 +2380,7 @@
         <v>5</v>
       </c>
       <c r="C77">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D77">
         <v>-0.2</v>
@@ -2505,7 +2397,7 @@
         <v>6</v>
       </c>
       <c r="C78">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -2522,13 +2414,13 @@
         <v>7</v>
       </c>
       <c r="C79">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="D79">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="E79">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2539,7 +2431,7 @@
         <v>8</v>
       </c>
       <c r="C80">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="D80">
         <v>4</v>
@@ -2556,10 +2448,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>32.9</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="D81">
-        <v>32.700000000000003</v>
+        <v>32.6</v>
       </c>
       <c r="E81">
         <v>32.5</v>
@@ -2573,13 +2465,13 @@
         <v>10</v>
       </c>
       <c r="C82">
-        <v>30.2</v>
+        <v>29.6</v>
       </c>
       <c r="D82">
-        <v>31.1</v>
+        <v>31.2</v>
       </c>
       <c r="E82">
-        <v>31.8</v>
+        <v>31.9</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,13 +2482,13 @@
         <v>11</v>
       </c>
       <c r="C83">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="D83">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E83">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,13 +2499,13 @@
         <v>12</v>
       </c>
       <c r="C84">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="D84">
-        <v>-1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="E84">
-        <v>-2.7</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2624,13 +2516,13 @@
         <v>13</v>
       </c>
       <c r="C85">
-        <v>14.4</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D85">
-        <v>-36.1</v>
+        <v>-39.299999999999997</v>
       </c>
       <c r="E85">
-        <v>-74.8</v>
+        <v>-76.8</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2641,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="C86">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="D86">
         <v>0.7</v>
@@ -2657,15 +2549,6 @@
       <c r="B87" t="s">
         <v>3</v>
       </c>
-      <c r="C87">
-        <v>30.2</v>
-      </c>
-      <c r="D87">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="E87">
-        <v>45.7</v>
-      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -2675,7 +2558,7 @@
         <v>4</v>
       </c>
       <c r="C88">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D88">
         <v>1.6</v>
@@ -2692,7 +2575,7 @@
         <v>5</v>
       </c>
       <c r="C89">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D89">
         <v>0.5</v>
@@ -2709,7 +2592,7 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D90">
         <v>1.1000000000000001</v>
@@ -2726,7 +2609,7 @@
         <v>7</v>
       </c>
       <c r="C91">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="D91">
         <v>3.6</v>
@@ -2743,7 +2626,7 @@
         <v>8</v>
       </c>
       <c r="C92">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="D92">
         <v>3.9</v>
@@ -2777,7 +2660,7 @@
         <v>10</v>
       </c>
       <c r="C94">
-        <v>24.5</v>
+        <v>24.6</v>
       </c>
       <c r="D94">
         <v>25.5</v>
@@ -2794,10 +2677,10 @@
         <v>11</v>
       </c>
       <c r="C95">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D95">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E95">
         <v>-0.4</v>
@@ -2811,7 +2694,7 @@
         <v>12</v>
       </c>
       <c r="C96">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -2828,13 +2711,13 @@
         <v>13</v>
       </c>
       <c r="C97">
-        <v>28.6</v>
+        <v>26.9</v>
       </c>
       <c r="D97">
-        <v>20.100000000000001</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="E97">
-        <v>26.1</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2845,7 +2728,7 @@
         <v>2</v>
       </c>
       <c r="C98">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="D98">
         <v>0.6</v>
@@ -2861,15 +2744,6 @@
       <c r="B99" t="s">
         <v>3</v>
       </c>
-      <c r="C99">
-        <v>34.1</v>
-      </c>
-      <c r="D99">
-        <v>43.1</v>
-      </c>
-      <c r="E99">
-        <v>51.5</v>
-      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -2879,7 +2753,7 @@
         <v>4</v>
       </c>
       <c r="C100">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="D100">
         <v>1.4</v>
@@ -2896,13 +2770,13 @@
         <v>5</v>
       </c>
       <c r="C101">
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D101">
         <v>0.4</v>
       </c>
       <c r="E101">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2930,7 +2804,7 @@
         <v>7</v>
       </c>
       <c r="C103">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="D103">
         <v>3.4</v>
@@ -2947,7 +2821,7 @@
         <v>8</v>
       </c>
       <c r="C104">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="D104">
         <v>4.2</v>
@@ -2964,10 +2838,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>34.4</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="D105">
-        <v>33.799999999999997</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="E105">
         <v>33.6</v>
@@ -2981,13 +2855,13 @@
         <v>10</v>
       </c>
       <c r="C106">
-        <v>33.700000000000003</v>
+        <v>33.9</v>
       </c>
       <c r="D106">
-        <v>35.5</v>
+        <v>35.6</v>
       </c>
       <c r="E106">
-        <v>36.9</v>
+        <v>37.1</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2998,13 +2872,13 @@
         <v>11</v>
       </c>
       <c r="C107">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="D107">
-        <v>-1.7</v>
+        <v>-1.8</v>
       </c>
       <c r="E107">
-        <v>-3.3</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,10 +2892,10 @@
         <v>1.5</v>
       </c>
       <c r="D108">
-        <v>2.2999999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="E108">
-        <v>5.2</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,13 +2906,13 @@
         <v>13</v>
       </c>
       <c r="C109">
-        <v>21.7</v>
+        <v>22</v>
       </c>
       <c r="D109">
-        <v>53.3</v>
+        <v>58.2</v>
       </c>
       <c r="E109">
-        <v>131.4</v>
+        <v>139.9</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3049,7 +2923,7 @@
         <v>2</v>
       </c>
       <c r="C110">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D110">
         <v>0.2</v>
@@ -3065,15 +2939,6 @@
       <c r="B111" t="s">
         <v>3</v>
       </c>
-      <c r="C111">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="D111">
-        <v>42.1</v>
-      </c>
-      <c r="E111">
-        <v>43</v>
-      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -3083,10 +2948,10 @@
         <v>4</v>
       </c>
       <c r="C112">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D112">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E112">
         <v>1.2</v>
@@ -3103,7 +2968,7 @@
         <v>0.2</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E113">
         <v>0.3</v>
@@ -3137,7 +3002,7 @@
         <v>3.1</v>
       </c>
       <c r="D115">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="E115">
         <v>3.2</v>
@@ -3171,7 +3036,7 @@
         <v>34.5</v>
       </c>
       <c r="D117">
-        <v>35.4</v>
+        <v>35.5</v>
       </c>
       <c r="E117">
         <v>35.299999999999997</v>
@@ -3185,7 +3050,7 @@
         <v>10</v>
       </c>
       <c r="C118">
-        <v>32</v>
+        <v>31.4</v>
       </c>
       <c r="D118">
         <v>32.5</v>
@@ -3202,7 +3067,7 @@
         <v>11</v>
       </c>
       <c r="C119">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="D119">
         <v>2.9</v>
@@ -3219,13 +3084,13 @@
         <v>12</v>
       </c>
       <c r="C120">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="D120">
-        <v>0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="E120">
-        <v>-2.7</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3236,13 +3101,13 @@
         <v>13</v>
       </c>
       <c r="C121">
-        <v>28.3</v>
+        <v>25.7</v>
       </c>
       <c r="D121">
-        <v>-16.7</v>
+        <v>-21.6</v>
       </c>
       <c r="E121">
-        <v>-81.5</v>
+        <v>-87</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3253,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="C122">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D122">
         <v>0.9</v>
@@ -3269,15 +3134,6 @@
       <c r="B123" t="s">
         <v>3</v>
       </c>
-      <c r="C123">
-        <v>28</v>
-      </c>
-      <c r="D123">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="E123">
-        <v>40.6</v>
-      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -3287,10 +3143,10 @@
         <v>4</v>
       </c>
       <c r="C124">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="D124">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E124">
         <v>2</v>
@@ -3304,7 +3160,7 @@
         <v>5</v>
       </c>
       <c r="C125">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="D125">
         <v>0.7</v>
@@ -3321,7 +3177,7 @@
         <v>6</v>
       </c>
       <c r="C126">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D126">
         <v>1.3</v>
@@ -3338,13 +3194,13 @@
         <v>7</v>
       </c>
       <c r="C127">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="D127">
         <v>4</v>
       </c>
       <c r="E127">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,7 +3211,7 @@
         <v>8</v>
       </c>
       <c r="C128">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="D128">
         <v>3.9</v>
@@ -3372,13 +3228,13 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>26.4</v>
+        <v>26.1</v>
       </c>
       <c r="D129">
         <v>25.8</v>
       </c>
       <c r="E129">
-        <v>25.7</v>
+        <v>25.6</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3389,7 +3245,7 @@
         <v>10</v>
       </c>
       <c r="C130">
-        <v>23.9</v>
+        <v>23.4</v>
       </c>
       <c r="D130">
         <v>23.8</v>
@@ -3406,10 +3262,10 @@
         <v>11</v>
       </c>
       <c r="C131">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="D131">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="E131">
         <v>1.5</v>
@@ -3423,13 +3279,13 @@
         <v>12</v>
       </c>
       <c r="C132">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="D132">
-        <v>-1</v>
+        <v>-1.2</v>
       </c>
       <c r="E132">
-        <v>-2.7</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3440,13 +3296,13 @@
         <v>13</v>
       </c>
       <c r="C133">
-        <v>3.5</v>
+        <v>-0.2</v>
       </c>
       <c r="D133">
-        <v>-38.700000000000003</v>
+        <v>-42</v>
       </c>
       <c r="E133">
-        <v>-76.5</v>
+        <v>-79.099999999999994</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3457,7 +3313,7 @@
         <v>2</v>
       </c>
       <c r="C134">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="D134">
         <v>0.4</v>
@@ -3473,15 +3329,6 @@
       <c r="B135" t="s">
         <v>3</v>
       </c>
-      <c r="C135">
-        <v>16.3</v>
-      </c>
-      <c r="D135">
-        <v>22.8</v>
-      </c>
-      <c r="E135">
-        <v>25.6</v>
-      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -3491,7 +3338,7 @@
         <v>4</v>
       </c>
       <c r="C136">
-        <v>2.2999999999999998</v>
+        <v>2</v>
       </c>
       <c r="D136">
         <v>1.2</v>
@@ -3507,15 +3354,6 @@
       <c r="B137" t="s">
         <v>5</v>
       </c>
-      <c r="C137" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="D137" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="E137" t="e">
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -3524,15 +3362,6 @@
       <c r="B138" t="s">
         <v>6</v>
       </c>
-      <c r="C138" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="D138" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="E138" t="e">
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3542,10 +3371,10 @@
         <v>7</v>
       </c>
       <c r="C139">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D139">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="E139">
         <v>3.5</v>
@@ -3559,7 +3388,7 @@
         <v>8</v>
       </c>
       <c r="C140">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="D140">
         <v>4.0999999999999996</v>
@@ -3576,7 +3405,7 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>54.9</v>
+        <v>53.2</v>
       </c>
       <c r="D141">
         <v>53.7</v>
@@ -3593,10 +3422,10 @@
         <v>10</v>
       </c>
       <c r="C142">
-        <v>57.6</v>
+        <v>57.8</v>
       </c>
       <c r="D142">
-        <v>59.5</v>
+        <v>59.6</v>
       </c>
       <c r="E142">
         <v>60.3</v>
@@ -3610,10 +3439,10 @@
         <v>11</v>
       </c>
       <c r="C143">
-        <v>-2.7</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="D143">
-        <v>-5.8</v>
+        <v>-5.9</v>
       </c>
       <c r="E143">
         <v>-6.6</v>
@@ -3627,13 +3456,13 @@
         <v>12</v>
       </c>
       <c r="C144">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="D144">
-        <v>7.1</v>
+        <v>7.7</v>
       </c>
       <c r="E144">
-        <v>15.1</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3644,13 +3473,13 @@
         <v>13</v>
       </c>
       <c r="C145">
-        <v>5.3</v>
+        <v>15.1</v>
       </c>
       <c r="D145">
-        <v>179.7</v>
+        <v>194.9</v>
       </c>
       <c r="E145">
-        <v>388.5</v>
+        <v>406.2</v>
       </c>
     </row>
   </sheetData>
@@ -3665,7 +3494,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,11 +3578,8 @@
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
+      <c r="B9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4039,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B803A11-2DAE-43BB-B2CB-37B5C05AD7C6}">
   <dimension ref="A1:CE34"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix tooltip rendering on language change.
</commit_message>
<xml_diff>
--- a/src/assets/years/2023.xlsx
+++ b/src/assets/years/2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\VanheR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7CD317-2F79-4EAE-B3D1-37E3038E7524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5398F7F-1608-42F7-908E-63833A68175E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3285" windowWidth="29040" windowHeight="15840" xr2:uid="{998BE1DA-C037-4508-8C33-93B2F93493F5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{998BE1DA-C037-4508-8C33-93B2F93493F5}"/>
   </bookViews>
   <sheets>
     <sheet name="VARS" sheetId="5" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="125">
   <si>
     <t>indicator</t>
   </si>
@@ -245,67 +245,22 @@
     <t>Content (French)</t>
   </si>
   <si>
-    <t>Current fiscal policy is marginally sustainable over the long term. Permanent tax decreases or spending increases amounting to 0.1 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Alberta currently spends less on health care (as a share of the provincial economy) than any other province. Thus, even once accounting for the cost pressures of population ageing, the province’s health care costs are projected to remain below those of some other provinces’ current health costs (as a share of the provincial economy).</t>
-  </si>
-  <si>
     <t>Current fiscal policy is not sustainable over the long term. Permanent tax increases or spending reductions amounting to 1.3 per cent of GDP ($5.1 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Because of relatively slower economic growth, we project that British Columbia will begin to receive Equalization entitlements beginning in 2052, with payments rising as a share of the provincial economy in later years.</t>
   </si>
   <si>
     <t>Current fiscal policy is not sustainable over the long term. Permanent tax increases or spending reductions amounting to 3.2 per cent of GDP ($2.9 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Because the province is projected to sustain above-average per capita economic growth, PBO projects that the province’s federal transfer revenue, including Equalization entitlements, will decline throughout the long term (as a share of the economy).</t>
-  </si>
-  <si>
-    <t>Current fiscal policy is marginally sustainable over the long term. Permanent tax decreases or spending increases amounting to 0.3 per cent of GDP ($0.1 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Federal transfers help to alleviate province’s long-term fiscal pressures due to raising health care costs. Over our long-term projection, federal transfers comprise a larger share of the economy in New Brunswick than any other province.</t>
-  </si>
-  <si>
-    <t>Current fiscal policy is marginally not sustainable over the long term. Modest, permanent tax increases or spending reductions amounting to 0.8 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Medium-term fiscal outlook of Newfoundland and Labrador positively contributes to ensuring fiscal sustainability. Rising health care costs due to population ageing are a key long-term fiscal pressure. Newfoundland and Labrador’s projected increase in health spending (as a share of the economy) is the largest of any province in PBO’s projection, except Prince Edward Island.</t>
-  </si>
-  <si>
     <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 1.0 per cent of GDP ($0.6 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Nova Scotia’s positive medium-term fiscal outlook contributes, in part, to ensuring fiscal sustainability. However, because Nova Scotia currently spends more on health care (as a share of the provincial economy) than the Canadian average and its population is projected to age more than the Canadian average, provincial health spending puts significant long-term fiscal pressure.</t>
-  </si>
-  <si>
-    <t>Current fiscal policy is marginally not sustainable over the long term. Modest, permanent tax increases or spending reductions amounting to 0.2 per cent of GDP ($1.8 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Ontario’s medium-term fiscal outlook positively contributes to ensuring fiscal sustainability. However, due to ageing population rising provincial health spending puts significant long-term fiscal pressure.</t>
   </si>
   <si>
     <t>Current fiscal policy is not sustainable over the long term. Permanent tax increases or spending reductions amounting to 2.4 per cent of GDP ($0.2 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Rising health care costs are the key long-term fiscal pressure. We project that Prince Edward Island will experience the largest (percentage-point) increase in health care spending in Canada due to population ageing and already high per-person spending on elderly health care.</t>
-  </si>
-  <si>
     <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 1.8 per cent of GDP ($10.0 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Provincial revenues exceed program spending throughout our projections. This relative stability in primary balance-to-GDP ratio primarily reflects rising Equalization and CHT transfers (relative to the size of Quebec’s economy) that largely offset increased health care spending.</t>
-  </si>
-  <si>
     <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 1.5 per cent of GDP ($1.6 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term</t>
-  </si>
-  <si>
-    <t>Saskatchewan currently spends less on health care (as a share of the provincial economy) than any other province, except for Alberta. Combined with the relatively modest population ageing and consequently the smallest (percentage-point) increase in health care spending in Canada, we project that Saskatchewan will experience the smallest increase in program spending.</t>
-  </si>
-  <si>
-    <t>Current fiscal policy is not sustainable over the long term. Permanent tax increases or spending reductions amounting to 6.4 per cent of GDP ($1.0 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
     <t xml:space="preserve">Because provincial-local government spending is growing more slowly in provinces than in the Territories in our projection, the Territorial Formula Financing does not keep pace with territorial program spending. We therefore project revenue declines (as a share of the economy) under the current formula. </t>
@@ -332,16 +287,7 @@
     <t>fsr_intro</t>
   </si>
   <si>
-    <t>The OPBO has prepared fact sheets for the provinces and territories.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
-  </si>
-  <si>
-    <t>Le BDPB a préparé des fiches d'information pour les provinces et les territoires.  Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
-  </si>
-  <si>
     <t>infographic_subsus_tl</t>
-  </si>
-  <si>
-    <t>Current fiscal policy in Quebec, Saskatchewa, Nova Scotia, New Brunswich and Alberta is **sustainable**.</t>
   </si>
   <si>
     <t>La politique financière actuelle au Québec, en Saskatchewan, en Nouvelle-Écosse, au Nouveau-Brunswick et en Alberta est **viable**.</t>
@@ -422,9 +368,6 @@
     <t>infographic_lt_perspective_ppp_legend</t>
   </si>
   <si>
-    <t>The current structure **are sustainable** over the long term.</t>
-  </si>
-  <si>
     <t>Les structures actuelles **sont viables** à long terme.</t>
   </si>
   <si>
@@ -455,22 +398,119 @@
     <t>Permanent changes in revenues or program spending required to stabilize debt-to-GDP ratio.</t>
   </si>
   <si>
-    <t>Modifications permanentes des prevenus ou des dépenses de programme nécessaires pour stabiliser le ratio de la dette au PIB.</t>
-  </si>
-  <si>
     <t>infographic_fg_neg_definition</t>
   </si>
   <si>
-    <t>Room available to inscrease spending or reduce taxes while maintaining fiscal sustainability.</t>
+    <t>Marge de manoeuvre permettant d'accroître les dépenses ou de réduire les impôts tout en assurant la viabilité financière.</t>
   </si>
   <si>
-    <t>Marge de manoeuvre permettant d'accroître les dépenses ou de réduire les impôts tout en assurant la viabilité financière.</t>
+    <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 0.1 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>Federal transfers are not projected to keep pace with Manitoba’s spending pressures. Because the province is projected to sustain above-average per capita economic growth, PBO projects that the province’s federal transfer revenue, including Equalization entitlements, will decline throughout the long term (as a share of the economy).</t>
+  </si>
+  <si>
+    <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 0.3 per cent of GDP ($0.1 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>Current fiscal policy is not sustainable over the long term. Modest, permanent tax increases or spending reductions amounting to 0.8 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>Medium-term fiscal outlook of Newfoundland and Labrador positively contributes to ensuring fiscal sustainability. However, rising health care costs due to population ageing are a key long-term fiscal pressure. With the least favourable differential between long-run effective interest rates and economic growth of any province, this will be a drag on its sustainability prospects.</t>
+  </si>
+  <si>
+    <t>Nova Scotia’s medium-term fiscal outlook positively contributes, in part, to it's fiscal sustainability. However, health care costs are Nova Scotia’s key long-term fiscal pressure. Nova Scotia currently spends more on health care (as a share of the provincial economy) than the Canadian average and its population is projected to age more than the Canadian average.</t>
+  </si>
+  <si>
+    <t>Current fiscal policy is not sustainable over the long term. Modest, permanent tax increases or spending reductions amounting to 0.2 per cent of GDP ($1.8 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>Ontario’s medium-term fiscal outlook positively contributes to ensuring fiscal sustainability. However, health care costs are Ontario’s key long-term fiscal pressure due to an ageing population.  With lower long-run effective interest rates than most other provinces, this contributes to a comparatively favourable differential between interest rates and economic growth, helping its sustainability prospects.</t>
+  </si>
+  <si>
+    <t>Provincial revenues exceed program spending throughout our projections. This relative stability in primary balance-to-GDP ratio primarily reflects rising transfer revenue, with increases to Equalization entitlements (relative to the size of the provincial economy) that largely offset increased health care spending.</t>
+  </si>
+  <si>
+    <t>Saskatchewan currently spends less on health care (as a share of the provincial economy) than any other province, except for Alberta. Combined with the relatively modest pressures from population ageing, and consequently the smallest (percentage-point) increase in health care spending in Canada, we project that Saskatchewan will experience the smallest increase in program spending (as a share of its economy).</t>
+  </si>
+  <si>
+    <t>Current fiscal policy is not sustainable over the long term. Permanent revenue increases or spending reductions amounting to 6.4 per cent of GDP ($1.0 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>Alberta's long-term outlook for total population growth is the highest in Canada. In the long run, Alberta will have the fastest growing economy. This is mainly due to favourable demographics resulting in higher total hours worked compared to the national average while labour productivity remains on par.</t>
+  </si>
+  <si>
+    <t>British Columbia’s long-term outlook for total population growth is in line with the national average. In the long run, British Columbia will have slower real GDP growth compared to the national average. This is mainly due to lower labour productivity compared to the national average.</t>
+  </si>
+  <si>
+    <t>Manitoba's long-term outlook for total population growth is in line with the national average. In the long run, Manitoba's real GDP growth will be slightly higher than the national average. This is mainly due to labour productivity catching up to and surpassing the national trend.</t>
+  </si>
+  <si>
+    <t>New Brunswick's long term outlook for total population growth is lower than the national average. In the long run, New Brunswick will have the slowest growing economy. This is mainly due to a faster growing older population putting downward pressure on total hours worked and lower labour productivity compared to the national average.</t>
+  </si>
+  <si>
+    <t>Newfoundland and Labrador's long term outlook for total population growth is the lowest in Canada. In the long run, Newfoundland and Labrador will have lower real GDP compared to the national average. This is mainly due to an aging population and slow population growth, and in spite of showcasing the highest levels of labour productivity growth in Canada.</t>
+  </si>
+  <si>
+    <t>Nova Scotia's long term outlook for total population growth is lower than the national average. In the long run, Nova Scotia's real GDP growth will be lower than the national average. This mainly due to having one of the lowest growth in total hours worked which in turn is attributable to a relatively older and aging population.</t>
+  </si>
+  <si>
+    <t>Ontario's long term outlook for total population growth is in line with the national average. In the long run, Ontario will have real GDP growth that is on par with the national average. This is mainly due to labour productivity growing slightly faster than the national average.</t>
+  </si>
+  <si>
+    <t>Prince Edward Island's long term outlook for total population growth is slightly below the national average. In the long run, Prince Edward Island will have lower real GDP growth compared to the national average. This is mainly due to slower population growth and population aging as well as lower labour productivity, though its overall outlook is favourable compared to the other Atlantic provinces.</t>
+  </si>
+  <si>
+    <t>Quebec's long term outlook for total population growth is lower than the national average. In the long run, Quebec's real GDP growth will be lower than the national average. This is mainly due to lower labour productivity and stagnant growth in total hours worked.</t>
+  </si>
+  <si>
+    <t>The territories' long term outlook for total population is below the national average, though its population is significantly younger. In the long run, the territories will have slightly lower real GDP growth compared to the national average. While the public sector is its most important industry, less favourable demographic conditions mainly explain lower economic growth compared to the national average.</t>
+  </si>
+  <si>
+    <t>Current fiscal policy in Quebec, Saskatchewan, Nova Scotia, New Brunswick and Alberta is **sustainable**.</t>
+  </si>
+  <si>
+    <t>The current structures **are sustainable** over the long term.</t>
+  </si>
+  <si>
+    <t>Modifications permanentes des revenus ou des dépenses de programme nécessaires pour stabiliser le ratio de la dette au PIB.</t>
+  </si>
+  <si>
+    <t>Room available to increase spending or reduce taxes while maintaining fiscal sustainability.</t>
+  </si>
+  <si>
+    <t>British Columbia's medium-term fiscal outlook negatively contributes to its fiscal sustainability as program spending exceeds provincial revenues. However, because of relatively slower economic growth, we project that British Columbia will begin to receive Equalization entitlements beginning in 2052, with payments rising as a share of the provincial economy in later years.</t>
+  </si>
+  <si>
+    <t>Federal transfers help to alleviate the province’s long-term fiscal pressures due to raising health care costs. Over our long-term projection, federal transfers comprise a larger share of the economy in New Brunswick than any other province.</t>
+  </si>
+  <si>
+    <t>Rising health care costs are the key long-term fiscal pressure. We project that Prince Edward Island will experience the largest (percentage-point) increase in health care spending in Canada due to already high spending on elderly health care on a per-person basis and that the province will experience greater-than-average population ageing.</t>
+  </si>
+  <si>
+    <t>Saskatchewan's long term outlook for total population growth is among the highest in Canada. In the long run, Saskatchewan will have one of the fastest growing economies. This is mainly due to favourable demographic conditions positively impacting  growth in total hours worked and hightened labour productivity compared to the national average and the other subnational levels.</t>
+  </si>
+  <si>
+    <t>The “At-a-Glance” tool visualizes and summarizes key drivers of fiscal sustainability for each province and territory over the long run from our latest Fiscal Sustainability Report. 
+The long-term fiscal projections are not forecasts or predictions of the most likely outcomes. They are illustrative scenarios that show the consequences of maintaining a government’s current fiscal policy over the long term, after accounting for the economic and fiscal implications of population ageing.
+We produce these projections to motivate discussion about the adequacy of current fiscal policy to deal with expected long-term demographic and economic challenges; the earlier that a required policy intervention can be identified, the lower will be the cost of its implementation.</t>
+  </si>
+  <si>
+    <t>L’outil « en un coup d’œil » permet de visualiser et de résumer les principaux facteurs de viabilité financière a long terme pour chaque province et territoire, d’après notre dernier rapport sur la viabilité financière. 
+Les projections budgétaires à long terme ne sont ni des prévisions ni des prédictions des résultats les plus probables. Ce sont plutôt des scénarios qui illustrent les conséquences du maintien de la politique budgétaire actuelle du gouvernement à long terme, après avoir pris en compte les répercussions économiques et financières du vieillissement de la population. 
+Ces projections visent à stimuler les discussions afin de déterminer si la politique budgétaire actuelle permet de relever adéquatement les défis à long terme sur les plans économiques et démographiques, car plus les interventions qui s’imposent seront faites rapidement, moins les coûts afférents seront élevés.</t>
+  </si>
+  <si>
+    <t>Except for British Columbia, Alberta holds less debt than all other provinces (as a share of the economy) with revenues exceeding program spending. PBO projects that Alberta will maintain the most favourable [differential between long-run effective interest rates and economic growth](## "Replace this with the content of a tooltip") of any province. These factors both positively contribute to Alberta’s sustainability prospects, despite the cost pressures of population ageing on the province’s health care spending.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,18 +528,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -514,16 +566,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7255F49-EEAA-44D0-BDAF-26A02A9AE815}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,223 +966,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>63</v>
+      <c r="B1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>2023</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>66</v>
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>70</v>
+        <v>53</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>79</v>
+        <v>59</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>85</v>
+        <v>65</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>88</v>
+        <v>68</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>91</v>
+        <v>71</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>96</v>
+        <v>76</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>100</v>
+        <v>80</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>104</v>
+        <v>83</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>107</v>
+        <v>86</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>110</v>
+        <v>89</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>113</v>
+        <v>91</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1134,13 +1197,14 @@
   <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J137" sqref="J137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1150,13 +1214,13 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="5">
         <v>2027</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="5">
         <v>2052</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="5">
         <v>2077</v>
       </c>
     </row>
@@ -1167,13 +1231,13 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>1.2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>0.6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>0.7</v>
       </c>
     </row>
@@ -1184,6 +1248,15 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="4">
+        <v>32.229999999999997</v>
+      </c>
+      <c r="D3" s="4">
+        <v>37.42</v>
+      </c>
+      <c r="E3" s="4">
+        <v>42.71</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1192,13 +1265,13 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>1.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>1.7</v>
       </c>
     </row>
@@ -1209,13 +1282,13 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>0.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -1226,13 +1299,13 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>1.2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1243,13 +1316,13 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>3.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>3.7</v>
       </c>
     </row>
@@ -1260,13 +1333,13 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>3.8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>3.9</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>3.9</v>
       </c>
     </row>
@@ -1277,13 +1350,13 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>26.9</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>26.4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>26</v>
       </c>
     </row>
@@ -1294,13 +1367,13 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>25.6</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>25.9</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>26</v>
       </c>
     </row>
@@ -1311,13 +1384,13 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>1.3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>0.4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1328,13 +1401,13 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>1.5</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>0.9</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -1345,13 +1418,13 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>19.2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>13.6</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>13.6</v>
       </c>
     </row>
@@ -1362,13 +1435,13 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>1.3</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>1.2</v>
       </c>
     </row>
@@ -1379,6 +1452,15 @@
       <c r="B15" t="s">
         <v>3</v>
       </c>
+      <c r="C15" s="4">
+        <v>24.94</v>
+      </c>
+      <c r="D15" s="4">
+        <v>30.92</v>
+      </c>
+      <c r="E15" s="4">
+        <v>36.17</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1387,13 +1469,13 @@
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>3.2</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>2.1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -1404,13 +1486,13 @@
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>2.1</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1421,13 +1503,13 @@
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>1.2</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1438,13 +1520,13 @@
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>5.3</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>4.2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>4.2</v>
       </c>
     </row>
@@ -1455,13 +1537,13 @@
       <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>3.6</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>3.9</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>3.9</v>
       </c>
     </row>
@@ -1472,13 +1554,13 @@
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>19.2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>19.100000000000001</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>19</v>
       </c>
     </row>
@@ -1489,13 +1571,13 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>18.2</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>18.7</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <v>19</v>
       </c>
     </row>
@@ -1506,13 +1588,13 @@
       <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>1</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>0.4</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>-0.1</v>
       </c>
     </row>
@@ -1523,13 +1605,13 @@
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>0.7</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="6">
         <v>-0.1</v>
       </c>
     </row>
@@ -1540,13 +1622,13 @@
       <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>2.7</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>-5</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <v>-4.8</v>
       </c>
     </row>
@@ -1557,13 +1639,13 @@
       <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>1.4</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>0.6</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -1574,6 +1656,15 @@
       <c r="B27" t="s">
         <v>3</v>
       </c>
+      <c r="C27" s="4">
+        <v>33.06</v>
+      </c>
+      <c r="D27" s="4">
+        <v>39.79</v>
+      </c>
+      <c r="E27" s="4">
+        <v>46.51</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1582,13 +1673,13 @@
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>1.9</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>0.9</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="6">
         <v>1.2</v>
       </c>
     </row>
@@ -1599,13 +1690,13 @@
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>1.2</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>0.3</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -1616,13 +1707,13 @@
       <c r="B30" t="s">
         <v>6</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>0.8</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>0.7</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <v>0.7</v>
       </c>
     </row>
@@ -1633,13 +1724,13 @@
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>3.9</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>2.9</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="6">
         <v>3.2</v>
       </c>
     </row>
@@ -1650,13 +1741,13 @@
       <c r="B32" t="s">
         <v>8</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>3.7</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>3.9</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="6">
         <v>3.9</v>
       </c>
     </row>
@@ -1667,13 +1758,13 @@
       <c r="B33" t="s">
         <v>9</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <v>25.2</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>25.5</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="6">
         <v>27</v>
       </c>
     </row>
@@ -1684,13 +1775,13 @@
       <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>26.2</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>27.1</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="6">
         <v>27.5</v>
       </c>
     </row>
@@ -1701,13 +1792,13 @@
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>-1</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>-1.6</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="6">
         <v>-0.5</v>
       </c>
     </row>
@@ -1718,13 +1809,13 @@
       <c r="B36" t="s">
         <v>12</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>2.8</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="6">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1735,13 +1826,13 @@
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>10.4</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="6">
         <v>65.900000000000006</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="6">
         <v>112.3</v>
       </c>
     </row>
@@ -1752,13 +1843,13 @@
       <c r="B38" t="s">
         <v>2</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="6">
         <v>0.8</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="6">
         <v>0.7</v>
       </c>
     </row>
@@ -1769,6 +1860,15 @@
       <c r="B39" t="s">
         <v>3</v>
       </c>
+      <c r="C39" s="4">
+        <v>38.39</v>
+      </c>
+      <c r="D39" s="4">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="E39" s="4">
+        <v>28.3</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1777,13 +1877,13 @@
       <c r="B40" t="s">
         <v>4</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>1.7</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="6">
         <v>1.8</v>
       </c>
     </row>
@@ -1794,13 +1894,13 @@
       <c r="B41" t="s">
         <v>5</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>1.2</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>0.6</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -1811,13 +1911,13 @@
       <c r="B42" t="s">
         <v>6</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <v>1.3</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>1.2</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="6">
         <v>1.2</v>
       </c>
     </row>
@@ -1828,13 +1928,13 @@
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="6">
         <v>3.7</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="6">
         <v>3.8</v>
       </c>
     </row>
@@ -1845,13 +1945,13 @@
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="6">
         <v>3.8</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="6">
         <v>4</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="6">
         <v>4</v>
       </c>
     </row>
@@ -1862,13 +1962,13 @@
       <c r="B45" t="s">
         <v>9</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="6">
         <v>30.9</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="6">
         <v>29.3</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="6">
         <v>28</v>
       </c>
     </row>
@@ -1879,13 +1979,13 @@
       <c r="B46" t="s">
         <v>10</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="6">
         <v>30.5</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="6">
         <v>31.5</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="6">
         <v>32.200000000000003</v>
       </c>
     </row>
@@ -1896,13 +1996,13 @@
       <c r="B47" t="s">
         <v>11</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="6">
         <v>0.4</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="6">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="6">
         <v>-4.2</v>
       </c>
     </row>
@@ -1913,13 +2013,13 @@
       <c r="B48" t="s">
         <v>12</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="6">
         <v>2.6</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="6">
         <v>3.7</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="6">
         <v>6.8</v>
       </c>
     </row>
@@ -1930,13 +2030,13 @@
       <c r="B49" t="s">
         <v>13</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="6">
         <v>36.299999999999997</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="6">
         <v>84.6</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="6">
         <v>177.1</v>
       </c>
     </row>
@@ -1947,13 +2047,13 @@
       <c r="B50" t="s">
         <v>2</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="6">
         <v>0.5</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="6">
         <v>0</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="6">
         <v>0.3</v>
       </c>
     </row>
@@ -1964,6 +2064,15 @@
       <c r="B51" t="s">
         <v>3</v>
       </c>
+      <c r="C51" s="7">
+        <v>40.47</v>
+      </c>
+      <c r="D51" s="7">
+        <v>44.94</v>
+      </c>
+      <c r="E51" s="7">
+        <v>49.01</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -1972,13 +2081,13 @@
       <c r="B52" t="s">
         <v>4</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="6">
         <v>1</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="6">
         <v>0.8</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1989,13 +2098,13 @@
       <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="6">
         <v>0.2</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="6">
         <v>-0.1</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="6">
         <v>0.2</v>
       </c>
     </row>
@@ -2006,13 +2115,13 @@
       <c r="B54" t="s">
         <v>6</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="6">
         <v>1</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="6">
         <v>0.9</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="6">
         <v>0.9</v>
       </c>
     </row>
@@ -2023,13 +2132,13 @@
       <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="6">
         <v>3.1</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="6">
         <v>2.8</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="6">
         <v>3.1</v>
       </c>
     </row>
@@ -2040,13 +2149,13 @@
       <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="6">
         <v>3.9</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="6">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -2057,13 +2166,13 @@
       <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="6">
         <v>32.9</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="6">
         <v>33.6</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="6">
         <v>33.6</v>
       </c>
     </row>
@@ -2074,13 +2183,13 @@
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="6">
         <v>31.1</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="6">
         <v>32.5</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="6">
         <v>32.9</v>
       </c>
     </row>
@@ -2091,13 +2200,13 @@
       <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="6">
         <v>1.8</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -2108,13 +2217,13 @@
       <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="6">
         <v>1.9</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="6">
         <v>0.8</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="6">
         <v>0.1</v>
       </c>
     </row>
@@ -2125,13 +2234,13 @@
       <c r="B61" t="s">
         <v>13</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="6">
         <v>18.399999999999999</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="6">
         <v>5.6</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="6">
         <v>-5.4</v>
       </c>
     </row>
@@ -2142,13 +2251,13 @@
       <c r="B62" t="s">
         <v>2</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="6">
         <v>-0.3</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="6">
         <v>-0.7</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="6">
         <v>-0.3</v>
       </c>
     </row>
@@ -2159,6 +2268,15 @@
       <c r="B63" t="s">
         <v>3</v>
       </c>
+      <c r="C63" s="4">
+        <v>44.04</v>
+      </c>
+      <c r="D63" s="4">
+        <v>54.61</v>
+      </c>
+      <c r="E63" s="4">
+        <v>59.06</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2167,13 +2285,13 @@
       <c r="B64" t="s">
         <v>4</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="6">
         <v>0.6</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="6">
         <v>0.8</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="6">
         <v>1.2</v>
       </c>
     </row>
@@ -2184,13 +2302,13 @@
       <c r="B65" t="s">
         <v>5</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="6">
         <v>-0.9</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="6">
         <v>-0.7</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="6">
         <v>-0.4</v>
       </c>
     </row>
@@ -2201,13 +2319,13 @@
       <c r="B66" t="s">
         <v>6</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="6">
         <v>1.7</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="6">
         <v>1.6</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="6">
         <v>1.6</v>
       </c>
     </row>
@@ -2218,13 +2336,13 @@
       <c r="B67" t="s">
         <v>7</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="6">
         <v>2.6</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="6">
         <v>2.8</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="6">
         <v>3.2</v>
       </c>
     </row>
@@ -2235,13 +2353,13 @@
       <c r="B68" t="s">
         <v>8</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="6">
         <v>3.9</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="6">
         <v>4.2</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="6">
         <v>4.2</v>
       </c>
     </row>
@@ -2252,13 +2370,13 @@
       <c r="B69" t="s">
         <v>9</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="6">
         <v>24</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="6">
         <v>23.8</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="6">
         <v>23.5</v>
       </c>
     </row>
@@ -2269,13 +2387,13 @@
       <c r="B70" t="s">
         <v>10</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="6">
         <v>22.2</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="6">
         <v>23.9</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="6">
         <v>24.1</v>
       </c>
     </row>
@@ -2286,13 +2404,13 @@
       <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="6">
         <v>1.8</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="6">
         <v>-0.1</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="6">
         <v>-0.6</v>
       </c>
     </row>
@@ -2303,13 +2421,13 @@
       <c r="B72" t="s">
         <v>12</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="6">
         <v>3.4</v>
       </c>
     </row>
@@ -2320,13 +2438,13 @@
       <c r="B73" t="s">
         <v>13</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="6">
         <v>30.4</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="6">
         <v>43.6</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="6">
         <v>78.8</v>
       </c>
     </row>
@@ -2337,13 +2455,13 @@
       <c r="B74" t="s">
         <v>2</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="6">
         <v>0.7</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="6">
         <v>0</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="6">
         <v>0.2</v>
       </c>
     </row>
@@ -2354,6 +2472,15 @@
       <c r="B75" t="s">
         <v>3</v>
       </c>
+      <c r="C75" s="4">
+        <v>37.99</v>
+      </c>
+      <c r="D75" s="4">
+        <v>42.74</v>
+      </c>
+      <c r="E75" s="4">
+        <v>50.61</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -2362,13 +2489,13 @@
       <c r="B76" t="s">
         <v>4</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="6">
         <v>1.4</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="6">
         <v>0.7</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -2379,13 +2506,13 @@
       <c r="B77" t="s">
         <v>5</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="6">
         <v>0.4</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="6">
         <v>-0.2</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="6">
         <v>0.1</v>
       </c>
     </row>
@@ -2396,13 +2523,13 @@
       <c r="B78" t="s">
         <v>6</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="6">
         <v>1</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2413,13 +2540,13 @@
       <c r="B79" t="s">
         <v>7</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="6">
         <v>3.4</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="6">
         <v>2.7</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="6">
         <v>3.2</v>
       </c>
     </row>
@@ -2430,13 +2557,13 @@
       <c r="B80" t="s">
         <v>8</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="6">
         <v>4</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="6">
         <v>4</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="6">
         <v>4</v>
       </c>
     </row>
@@ -2447,13 +2574,13 @@
       <c r="B81" t="s">
         <v>9</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="6">
         <v>32.700000000000003</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="6">
         <v>32.6</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="6">
         <v>32.5</v>
       </c>
     </row>
@@ -2464,13 +2591,13 @@
       <c r="B82" t="s">
         <v>10</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="6">
         <v>29.6</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="6">
         <v>31.2</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="6">
         <v>31.9</v>
       </c>
     </row>
@@ -2481,13 +2608,13 @@
       <c r="B83" t="s">
         <v>11</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="6">
         <v>3.1</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="6">
         <v>1.5</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -2498,13 +2625,13 @@
       <c r="B84" t="s">
         <v>12</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="6">
         <v>1.2</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="6">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="6">
         <v>-2.8</v>
       </c>
     </row>
@@ -2515,13 +2642,13 @@
       <c r="B85" t="s">
         <v>13</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="6">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="6">
         <v>-39.299999999999997</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="6">
         <v>-76.8</v>
       </c>
     </row>
@@ -2532,13 +2659,13 @@
       <c r="B86" t="s">
         <v>2</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="6">
         <v>1.3</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="6">
         <v>0.7</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="6">
         <v>0.7</v>
       </c>
     </row>
@@ -2549,6 +2676,15 @@
       <c r="B87" t="s">
         <v>3</v>
       </c>
+      <c r="C87" s="4">
+        <v>31.08</v>
+      </c>
+      <c r="D87" s="4">
+        <v>36.74</v>
+      </c>
+      <c r="E87" s="4">
+        <v>43.7</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -2557,13 +2693,13 @@
       <c r="B88" t="s">
         <v>4</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="6">
         <v>1.6</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="6">
         <v>1.8</v>
       </c>
     </row>
@@ -2574,13 +2710,13 @@
       <c r="B89" t="s">
         <v>5</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="6">
         <v>0.5</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -2591,13 +2727,13 @@
       <c r="B90" t="s">
         <v>6</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="6">
         <v>1.2</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -2608,13 +2744,13 @@
       <c r="B91" t="s">
         <v>7</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="6">
         <v>4.2</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="6">
         <v>3.6</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="6">
         <v>3.8</v>
       </c>
     </row>
@@ -2625,13 +2761,13 @@
       <c r="B92" t="s">
         <v>8</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="6">
         <v>3.7</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="6">
         <v>3.9</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="6">
         <v>3.9</v>
       </c>
     </row>
@@ -2642,13 +2778,13 @@
       <c r="B93" t="s">
         <v>9</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="6">
         <v>25.8</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="6">
         <v>25.6</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="6">
         <v>25.5</v>
       </c>
     </row>
@@ -2659,13 +2795,13 @@
       <c r="B94" t="s">
         <v>10</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="6">
         <v>24.6</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="6">
         <v>25.5</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="6">
         <v>25.9</v>
       </c>
     </row>
@@ -2676,13 +2812,13 @@
       <c r="B95" t="s">
         <v>11</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="6">
         <v>1.2</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="6">
         <v>0.1</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="6">
         <v>-0.4</v>
       </c>
     </row>
@@ -2693,13 +2829,13 @@
       <c r="B96" t="s">
         <v>12</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="6">
         <v>1.5</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="6">
         <v>1</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -2710,13 +2846,13 @@
       <c r="B97" t="s">
         <v>13</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="6">
         <v>26.9</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="6">
         <v>20.399999999999999</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="6">
         <v>27.2</v>
       </c>
     </row>
@@ -2727,13 +2863,13 @@
       <c r="B98" t="s">
         <v>2</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="6">
         <v>1.2</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="6">
         <v>0.6</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -2744,6 +2880,15 @@
       <c r="B99" t="s">
         <v>3</v>
       </c>
+      <c r="C99" s="4">
+        <v>33.69</v>
+      </c>
+      <c r="D99" s="4">
+        <v>39.53</v>
+      </c>
+      <c r="E99" s="4">
+        <v>50.51</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -2752,13 +2897,13 @@
       <c r="B100" t="s">
         <v>4</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="6">
         <v>2.1</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="6">
         <v>1.4</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="6">
         <v>1.6</v>
       </c>
     </row>
@@ -2769,13 +2914,13 @@
       <c r="B101" t="s">
         <v>5</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="6">
         <v>0.4</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="6">
         <v>0.6</v>
       </c>
     </row>
@@ -2786,13 +2931,13 @@
       <c r="B102" t="s">
         <v>6</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="6">
         <v>1.2</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2803,13 +2948,13 @@
       <c r="B103" t="s">
         <v>7</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="6">
         <v>4.2</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="6">
         <v>3.4</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="6">
         <v>3.6</v>
       </c>
     </row>
@@ -2820,13 +2965,13 @@
       <c r="B104" t="s">
         <v>8</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="6">
         <v>4</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="6">
         <v>4.2</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="6">
         <v>4.2</v>
       </c>
     </row>
@@ -2837,13 +2982,13 @@
       <c r="B105" t="s">
         <v>9</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="6">
         <v>34.200000000000003</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="6">
         <v>33.700000000000003</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="6">
         <v>33.6</v>
       </c>
     </row>
@@ -2854,13 +2999,13 @@
       <c r="B106" t="s">
         <v>10</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="6">
         <v>33.9</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="6">
         <v>35.6</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="6">
         <v>37.1</v>
       </c>
     </row>
@@ -2871,13 +3016,13 @@
       <c r="B107" t="s">
         <v>11</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="6">
         <v>0.3</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="6">
         <v>-1.8</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="6">
         <v>-3.5</v>
       </c>
     </row>
@@ -2888,13 +3033,13 @@
       <c r="B108" t="s">
         <v>12</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="6">
         <v>1.5</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="6">
         <v>2.5</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="6">
         <v>5.5</v>
       </c>
     </row>
@@ -2905,13 +3050,13 @@
       <c r="B109" t="s">
         <v>13</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="6">
         <v>22</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="6">
         <v>58.2</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="6">
         <v>139.9</v>
       </c>
     </row>
@@ -2922,13 +3067,13 @@
       <c r="B110" t="s">
         <v>2</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="6">
         <v>0.5</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="6">
         <v>0.2</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="6">
         <v>0.4</v>
       </c>
     </row>
@@ -2939,6 +3084,15 @@
       <c r="B111" t="s">
         <v>3</v>
       </c>
+      <c r="C111" s="4">
+        <v>37.380000000000003</v>
+      </c>
+      <c r="D111" s="4">
+        <v>42.58</v>
+      </c>
+      <c r="E111" s="4">
+        <v>44.03</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -2947,13 +3101,13 @@
       <c r="B112" t="s">
         <v>4</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="6">
         <v>1</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="6">
         <v>0.9</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="6">
         <v>1.2</v>
       </c>
     </row>
@@ -2964,13 +3118,13 @@
       <c r="B113" t="s">
         <v>5</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="6">
         <v>0.2</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="6">
         <v>0.1</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="6">
         <v>0.3</v>
       </c>
     </row>
@@ -2981,13 +3135,13 @@
       <c r="B114" t="s">
         <v>6</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="6">
         <v>1</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="6">
         <v>0.9</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="6">
         <v>0.8</v>
       </c>
     </row>
@@ -2998,13 +3152,13 @@
       <c r="B115" t="s">
         <v>7</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="6">
         <v>3.1</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="6">
         <v>2.9</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="6">
         <v>3.2</v>
       </c>
     </row>
@@ -3015,13 +3169,13 @@
       <c r="B116" t="s">
         <v>8</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="6">
         <v>4</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="6">
         <v>4</v>
       </c>
     </row>
@@ -3032,13 +3186,13 @@
       <c r="B117" t="s">
         <v>9</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="6">
         <v>34.5</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="6">
         <v>35.5</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="6">
         <v>35.299999999999997</v>
       </c>
     </row>
@@ -3049,13 +3203,13 @@
       <c r="B118" t="s">
         <v>10</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="6">
         <v>31.4</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="6">
         <v>32.5</v>
       </c>
-      <c r="E118">
+      <c r="E118" s="6">
         <v>32.799999999999997</v>
       </c>
     </row>
@@ -3066,13 +3220,13 @@
       <c r="B119" t="s">
         <v>11</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="6">
         <v>3.2</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="6">
         <v>2.9</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="6">
         <v>2.5</v>
       </c>
     </row>
@@ -3083,13 +3237,13 @@
       <c r="B120" t="s">
         <v>12</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="6">
         <v>2.5</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="6">
         <v>-0.1</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="6">
         <v>-2.9</v>
       </c>
     </row>
@@ -3100,13 +3254,13 @@
       <c r="B121" t="s">
         <v>13</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="6">
         <v>25.7</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="6">
         <v>-21.6</v>
       </c>
-      <c r="E121">
+      <c r="E121" s="6">
         <v>-87</v>
       </c>
     </row>
@@ -3117,13 +3271,13 @@
       <c r="B122" t="s">
         <v>2</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="6">
         <v>1.3</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="6">
         <v>0.9</v>
       </c>
-      <c r="E122">
+      <c r="E122" s="6">
         <v>0.8</v>
       </c>
     </row>
@@ -3134,6 +3288,15 @@
       <c r="B123" t="s">
         <v>3</v>
       </c>
+      <c r="C123" s="4">
+        <v>29.25</v>
+      </c>
+      <c r="D123" s="4">
+        <v>32.31</v>
+      </c>
+      <c r="E123" s="4">
+        <v>38.17</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -3142,13 +3305,13 @@
       <c r="B124" t="s">
         <v>4</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="6">
         <v>2.7</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="6">
         <v>2</v>
       </c>
-      <c r="E124">
+      <c r="E124" s="6">
         <v>2</v>
       </c>
     </row>
@@ -3159,13 +3322,13 @@
       <c r="B125" t="s">
         <v>5</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="6">
         <v>1.4</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="6">
         <v>0.7</v>
       </c>
-      <c r="E125">
+      <c r="E125" s="6">
         <v>0.7</v>
       </c>
     </row>
@@ -3176,13 +3339,13 @@
       <c r="B126" t="s">
         <v>6</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="6">
         <v>1.4</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="6">
         <v>1.3</v>
       </c>
-      <c r="E126">
+      <c r="E126" s="6">
         <v>1.3</v>
       </c>
     </row>
@@ -3193,13 +3356,13 @@
       <c r="B127" t="s">
         <v>7</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="6">
         <v>4.7</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="6">
         <v>4</v>
       </c>
-      <c r="E127">
+      <c r="E127" s="6">
         <v>4</v>
       </c>
     </row>
@@ -3210,13 +3373,13 @@
       <c r="B128" t="s">
         <v>8</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="6">
         <v>3.6</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="6">
         <v>3.9</v>
       </c>
-      <c r="E128">
+      <c r="E128" s="6">
         <v>3.9</v>
       </c>
     </row>
@@ -3227,13 +3390,13 @@
       <c r="B129" t="s">
         <v>9</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="6">
         <v>26.1</v>
       </c>
-      <c r="D129">
+      <c r="D129" s="6">
         <v>25.8</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="6">
         <v>25.6</v>
       </c>
     </row>
@@ -3244,13 +3407,13 @@
       <c r="B130" t="s">
         <v>10</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="6">
         <v>23.4</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="6">
         <v>23.8</v>
       </c>
-      <c r="E130">
+      <c r="E130" s="6">
         <v>24.1</v>
       </c>
     </row>
@@ -3261,13 +3424,13 @@
       <c r="B131" t="s">
         <v>11</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="6">
         <v>2.6</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="6">
         <v>2</v>
       </c>
-      <c r="E131">
+      <c r="E131" s="6">
         <v>1.5</v>
       </c>
     </row>
@@ -3278,13 +3441,13 @@
       <c r="B132" t="s">
         <v>12</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="6">
         <v>0.9</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="6">
         <v>-1.2</v>
       </c>
-      <c r="E132">
+      <c r="E132" s="6">
         <v>-2.8</v>
       </c>
     </row>
@@ -3295,13 +3458,13 @@
       <c r="B133" t="s">
         <v>13</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="6">
         <v>-0.2</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="6">
         <v>-42</v>
       </c>
-      <c r="E133">
+      <c r="E133" s="6">
         <v>-79.099999999999994</v>
       </c>
     </row>
@@ -3312,13 +3475,13 @@
       <c r="B134" t="s">
         <v>2</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="6">
         <v>0.9</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="6">
         <v>0.4</v>
       </c>
-      <c r="E134">
+      <c r="E134" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -3329,6 +3492,15 @@
       <c r="B135" t="s">
         <v>3</v>
       </c>
+      <c r="C135" s="4">
+        <v>17.41</v>
+      </c>
+      <c r="D135" s="4">
+        <v>23.62</v>
+      </c>
+      <c r="E135" s="4">
+        <v>25.51</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -3337,13 +3509,13 @@
       <c r="B136" t="s">
         <v>4</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="6">
         <v>2</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="6">
         <v>1.2</v>
       </c>
-      <c r="E136">
+      <c r="E136" s="6">
         <v>1.5</v>
       </c>
     </row>
@@ -3354,6 +3526,9 @@
       <c r="B137" t="s">
         <v>5</v>
       </c>
+      <c r="C137" s="8"/>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -3362,6 +3537,9 @@
       <c r="B138" t="s">
         <v>6</v>
       </c>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -3370,13 +3548,13 @@
       <c r="B139" t="s">
         <v>7</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="6">
         <v>3.3</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="6">
         <v>3.5</v>
       </c>
     </row>
@@ -3387,13 +3565,13 @@
       <c r="B140" t="s">
         <v>8</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="6">
         <v>4</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="6">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -3404,13 +3582,13 @@
       <c r="B141" t="s">
         <v>9</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="6">
         <v>53.2</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="6">
         <v>53.7</v>
       </c>
-      <c r="E141">
+      <c r="E141" s="6">
         <v>53.7</v>
       </c>
     </row>
@@ -3421,13 +3599,13 @@
       <c r="B142" t="s">
         <v>10</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="6">
         <v>57.8</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="6">
         <v>59.6</v>
       </c>
-      <c r="E142">
+      <c r="E142" s="6">
         <v>60.3</v>
       </c>
     </row>
@@ -3438,13 +3616,13 @@
       <c r="B143" t="s">
         <v>11</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="6">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="6">
         <v>-5.9</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="6">
         <v>-6.6</v>
       </c>
     </row>
@@ -3455,13 +3633,13 @@
       <c r="B144" t="s">
         <v>12</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="6">
         <v>1.2</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="6">
         <v>7.7</v>
       </c>
-      <c r="E144">
+      <c r="E144" s="6">
         <v>15.7</v>
       </c>
     </row>
@@ -3472,13 +3650,13 @@
       <c r="B145" t="s">
         <v>13</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="6">
         <v>15.1</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="6">
         <v>194.9</v>
       </c>
-      <c r="E145">
+      <c r="E145" s="6">
         <v>406.2</v>
       </c>
     </row>
@@ -3615,10 +3793,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C496FAE6-5834-4DFC-B56D-04D2AE526F4F}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,215 +3821,304 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="B5" s="10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B8" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B26" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B29" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B31" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B32" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>61</v>
+      <c r="B34" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rounded to 1 decimal all numbers.
</commit_message>
<xml_diff>
--- a/src/assets/years/2023.xlsx
+++ b/src/assets/years/2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MalanC\AppData\Roaming\OpenText\OTEdit\EC_pbodocs\c732605\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5398F7F-1608-42F7-908E-63833A68175E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E79BAD-0EA7-48B3-9BCB-34F1916039E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{998BE1DA-C037-4508-8C33-93B2F93493F5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18856" windowHeight="13875" activeTab="1" xr2:uid="{998BE1DA-C037-4508-8C33-93B2F93493F5}"/>
   </bookViews>
   <sheets>
     <sheet name="VARS" sheetId="5" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="131">
   <si>
     <t>indicator</t>
   </si>
@@ -206,21 +206,6 @@
     <t>is_sustainable</t>
   </si>
   <si>
-    <t>Nous prévoyons que la croissance du PIB réel de la Colombie-Britannique sera inférieure à la moyenne...</t>
-  </si>
-  <si>
-    <t>Par conséquent, la politique budgétaire actuelle n'est pas viable à long terme....</t>
-  </si>
-  <si>
-    <t>Lorem ipsum…</t>
-  </si>
-  <si>
-    <t> Integer nec nunc ac odio *pharetra* venenati.</t>
-  </si>
-  <si>
-    <t>Lorem [ipsum](https://www.example.com)…</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -260,12 +245,6 @@
     <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 1.8 per cent of GDP ($10.0 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 1.5 per cent of GDP ($1.6 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Because provincial-local government spending is growing more slowly in provinces than in the Territories in our projection, the Territorial Formula Financing does not keep pace with territorial program spending. We therefore project revenue declines (as a share of the economy) under the current formula. </t>
-  </si>
-  <si>
     <t>Value (or en)</t>
   </si>
   <si>
@@ -407,27 +386,9 @@
     <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 0.1 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Federal transfers are not projected to keep pace with Manitoba’s spending pressures. Because the province is projected to sustain above-average per capita economic growth, PBO projects that the province’s federal transfer revenue, including Equalization entitlements, will decline throughout the long term (as a share of the economy).</t>
-  </si>
-  <si>
     <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 0.3 per cent of GDP ($0.1 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Current fiscal policy is not sustainable over the long term. Modest, permanent tax increases or spending reductions amounting to 0.8 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Medium-term fiscal outlook of Newfoundland and Labrador positively contributes to ensuring fiscal sustainability. However, rising health care costs due to population ageing are a key long-term fiscal pressure. With the least favourable differential between long-run effective interest rates and economic growth of any province, this will be a drag on its sustainability prospects.</t>
-  </si>
-  <si>
-    <t>Nova Scotia’s medium-term fiscal outlook positively contributes, in part, to it's fiscal sustainability. However, health care costs are Nova Scotia’s key long-term fiscal pressure. Nova Scotia currently spends more on health care (as a share of the provincial economy) than the Canadian average and its population is projected to age more than the Canadian average.</t>
-  </si>
-  <si>
-    <t>Current fiscal policy is not sustainable over the long term. Modest, permanent tax increases or spending reductions amounting to 0.2 per cent of GDP ($1.8 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
-  </si>
-  <si>
-    <t>Ontario’s medium-term fiscal outlook positively contributes to ensuring fiscal sustainability. However, health care costs are Ontario’s key long-term fiscal pressure due to an ageing population.  With lower long-run effective interest rates than most other provinces, this contributes to a comparatively favourable differential between interest rates and economic growth, helping its sustainability prospects.</t>
-  </si>
-  <si>
     <t>Provincial revenues exceed program spending throughout our projections. This relative stability in primary balance-to-GDP ratio primarily reflects rising transfer revenue, with increases to Equalization entitlements (relative to the size of the provincial economy) that largely offset increased health care spending.</t>
   </si>
   <si>
@@ -437,36 +398,6 @@
     <t>Current fiscal policy is not sustainable over the long term. Permanent revenue increases or spending reductions amounting to 6.4 per cent of GDP ($1.0 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
   </si>
   <si>
-    <t>Alberta's long-term outlook for total population growth is the highest in Canada. In the long run, Alberta will have the fastest growing economy. This is mainly due to favourable demographics resulting in higher total hours worked compared to the national average while labour productivity remains on par.</t>
-  </si>
-  <si>
-    <t>British Columbia’s long-term outlook for total population growth is in line with the national average. In the long run, British Columbia will have slower real GDP growth compared to the national average. This is mainly due to lower labour productivity compared to the national average.</t>
-  </si>
-  <si>
-    <t>Manitoba's long-term outlook for total population growth is in line with the national average. In the long run, Manitoba's real GDP growth will be slightly higher than the national average. This is mainly due to labour productivity catching up to and surpassing the national trend.</t>
-  </si>
-  <si>
-    <t>New Brunswick's long term outlook for total population growth is lower than the national average. In the long run, New Brunswick will have the slowest growing economy. This is mainly due to a faster growing older population putting downward pressure on total hours worked and lower labour productivity compared to the national average.</t>
-  </si>
-  <si>
-    <t>Newfoundland and Labrador's long term outlook for total population growth is the lowest in Canada. In the long run, Newfoundland and Labrador will have lower real GDP compared to the national average. This is mainly due to an aging population and slow population growth, and in spite of showcasing the highest levels of labour productivity growth in Canada.</t>
-  </si>
-  <si>
-    <t>Nova Scotia's long term outlook for total population growth is lower than the national average. In the long run, Nova Scotia's real GDP growth will be lower than the national average. This mainly due to having one of the lowest growth in total hours worked which in turn is attributable to a relatively older and aging population.</t>
-  </si>
-  <si>
-    <t>Ontario's long term outlook for total population growth is in line with the national average. In the long run, Ontario will have real GDP growth that is on par with the national average. This is mainly due to labour productivity growing slightly faster than the national average.</t>
-  </si>
-  <si>
-    <t>Prince Edward Island's long term outlook for total population growth is slightly below the national average. In the long run, Prince Edward Island will have lower real GDP growth compared to the national average. This is mainly due to slower population growth and population aging as well as lower labour productivity, though its overall outlook is favourable compared to the other Atlantic provinces.</t>
-  </si>
-  <si>
-    <t>Quebec's long term outlook for total population growth is lower than the national average. In the long run, Quebec's real GDP growth will be lower than the national average. This is mainly due to lower labour productivity and stagnant growth in total hours worked.</t>
-  </si>
-  <si>
-    <t>The territories' long term outlook for total population is below the national average, though its population is significantly younger. In the long run, the territories will have slightly lower real GDP growth compared to the national average. While the public sector is its most important industry, less favourable demographic conditions mainly explain lower economic growth compared to the national average.</t>
-  </si>
-  <si>
     <t>Current fiscal policy in Quebec, Saskatchewan, Nova Scotia, New Brunswick and Alberta is **sustainable**.</t>
   </si>
   <si>
@@ -479,16 +410,7 @@
     <t>Room available to increase spending or reduce taxes while maintaining fiscal sustainability.</t>
   </si>
   <si>
-    <t>British Columbia's medium-term fiscal outlook negatively contributes to its fiscal sustainability as program spending exceeds provincial revenues. However, because of relatively slower economic growth, we project that British Columbia will begin to receive Equalization entitlements beginning in 2052, with payments rising as a share of the provincial economy in later years.</t>
-  </si>
-  <si>
-    <t>Federal transfers help to alleviate the province’s long-term fiscal pressures due to raising health care costs. Over our long-term projection, federal transfers comprise a larger share of the economy in New Brunswick than any other province.</t>
-  </si>
-  <si>
     <t>Rising health care costs are the key long-term fiscal pressure. We project that Prince Edward Island will experience the largest (percentage-point) increase in health care spending in Canada due to already high spending on elderly health care on a per-person basis and that the province will experience greater-than-average population ageing.</t>
-  </si>
-  <si>
-    <t>Saskatchewan's long term outlook for total population growth is among the highest in Canada. In the long run, Saskatchewan will have one of the fastest growing economies. This is mainly due to favourable demographic conditions positively impacting  growth in total hours worked and hightened labour productivity compared to the national average and the other subnational levels.</t>
   </si>
   <si>
     <t>The “At-a-Glance” tool visualizes and summarizes key drivers of fiscal sustainability for each province and territory over the long run from our latest Fiscal Sustainability Report. 
@@ -501,7 +423,103 @@
 Ces projections visent à stimuler les discussions afin de déterminer si la politique budgétaire actuelle permet de relever adéquatement les défis à long terme sur les plans économiques et démographiques, car plus les interventions qui s’imposent seront faites rapidement, moins les coûts afférents seront élevés.</t>
   </si>
   <si>
-    <t>Except for British Columbia, Alberta holds less debt than all other provinces (as a share of the economy) with revenues exceeding program spending. PBO projects that Alberta will maintain the most favourable [differential between long-run effective interest rates and economic growth](## "Replace this with the content of a tooltip") of any province. These factors both positively contribute to Alberta’s sustainability prospects, despite the cost pressures of population ageing on the province’s health care spending.</t>
+    <t>Current fiscal policy is sustainable over the long term. Permanent tax decreases or spending increases amounting to 1.5 per cent of GDP ($1.6 billion in current dollars, growing in line with GDP thereafter) would be possible, while stabilizing government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle n'est pas viable à long terme. Des hausses d’impôts ou des réductions de dépenses permanentes représentant 1,3 % du PIB (5,1 milliards de dollars, en dollars courants, augmentant en fonction du PIB par la suite) seraient nécessaires pour stabiliser la dette nette du gouvernement à long terme (en proportion de l’économie).</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle n'est pas viable à long terme. Des hausses d’impôts ou des réductions de dépenses permanentes représentant 3,2 % du PIB (2,9 milliards de dollars, en dollars courants, augmentant en fonction du PIB par la suite) seraient nécessaires pour stabiliser la dette nette du gouvernement à long terme (en proportion de l’économie).</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle est viable à long terme. La province pourrait réduire ses impôts ou augmenter ses dépenses de façon permanente à raison de 0,1 % du PIB (0,3 milliards de dollars, en dollars courants, augmentant ensuite au rythme du PIB) tout en stabilisant la dette nette du gouvernement (en pourcentage de l’économie) à long terme.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle est viable à long terme. La province pourrait réduire ses impôts ou augmenter ses dépenses de façon permanente à raison de 0,3 % du PIB (0,1 milliards de dollars, en dollars courants, augmentant ensuite au rythme du PIB) tout en stabilisant la dette nette du gouvernement (en pourcentage de l’économie) à long terme.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle est viable à long terme. La province pourrait réduire ses impôts ou augmenter ses dépenses de façon permanente à raison de 1,0 % du PIB (0,6 milliards de dollars, en dollars courants, augmentant ensuite au rythme du PIB) tout en stabilisant la dette nette du gouvernement (en pourcentage de l’économie) à long terme.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle n'est pas viable à long terme. Des hausses d’impôts ou des réductions de dépenses permanentes représentant 2,4 % du PIB (0,2 milliards de dollars, en dollars courants, augmentant en fonction du PIB par la suite) seraient nécessaires pour stabiliser la dette nette du gouvernement à long terme (en proportion de l’économie).</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle est viable à long terme. La province pourrait réduire ses impôts ou augmenter ses dépenses de façon permanente à raison de 1,8 % du PIB (10,0 milliards de dollars, en dollars courants, augmentant ensuite au rythme du PIB) tout en stabilisant la dette nette du gouvernement (en pourcentage de l’économie) à long terme.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle est viable à long terme. La province pourrait réduire ses impôts ou augmenter ses dépenses de façon permanente à raison de 1,5 % du PIB (1,6 milliards de dollars, en dollars courants, augmentant ensuite au rythme du PIB) tout en stabilisant la dette nette du gouvernement (en pourcentage de l’économie) à long terme.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle n'est pas viable à long terme. Des hausses d’impôts ou des réductions de dépenses permanentes représentant 6,4 % du PIB (1,0 milliards de dollars, en dollars courants, augmentant en fonction du PIB par la suite) seraient nécessaires pour stabiliser la dette nette du gouvernement à long terme (en proportion de l’économie).</t>
+  </si>
+  <si>
+    <t>Alberta’s long-run fiscal outlook begins favourably – current revenues significantly exceed current spending as a share of the economy. However, due to provincial medium-term plans and cost pressures of population ageing the primary balances are projected to deteriorate over the projection horizon.</t>
+  </si>
+  <si>
+    <t>British Columbia's medium-term fiscal outlook negatively contributes to its fiscal sustainability as program spending significantly exceeds provincial revenues as a share of GDP. However, because of relatively slower economic growth, we project that British Columbia will begin to receive Equalization beginning in 2052, with payments rising as a share of the provincial economy in later years, helping to improve the primary balance over the long term.</t>
+  </si>
+  <si>
+    <t>Federal transfers are not projected to keep pace with Manitoba’s spending pressures. Because the province is projected to sustain above-average real GDP per capita growth, the province’s federal transfer revenue, including Equalization payments, will decline over the long term as a share of the economy.</t>
+  </si>
+  <si>
+    <t>Growth in federal transfers relative to the size of New Brunswick’s economy help to alleviate long-term fiscal pressures due to rising health care costs. Over our long-term projection, federal transfers comprise a larger share of the economy in New Brunswick than any other province.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newfoundland and Labrador's medium-term fiscal outlook positively contributes to fiscal sustainability. However, rising health care costs due to population ageing and declining federal transfers (as a share of the economy) are key long-term fiscal pressures. </t>
+  </si>
+  <si>
+    <t>Nova Scotia’s medium-term fiscal outlook positively contributes to its fiscal sustainability. However, health care costs are Nova Scotia’s key long-term fiscal pressure. Nova Scotia currently spends more on health care (as a share of the provincial economy) than the Canadian average and its population is projected to age more than the Canadian average.</t>
+  </si>
+  <si>
+    <t>Ontario’s medium-term fiscal outlook positively contributes to ensuring fiscal sustainability. However, health care costs are Ontario’s key long-term fiscal pressure due to an ageing population, which are compounded by declining federal transfers (as a share of the economy).</t>
+  </si>
+  <si>
+    <t>The territories’ initial fiscal position is not favourable to fiscal sustainability – current revenues fall well short of program spending as a share of the economy. Further, due to population ageing cost pressures, their primary balances are projected to deteriorate further over the projection horizon.</t>
+  </si>
+  <si>
+    <t>Current fiscal policy is not sustainable over the long term. Permanent tax increases or spending reductions amounting to 0.8 per cent of GDP ($0.3 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle n'est pas viable à long terme. Des hausses d’impôts ou des réductions de dépenses permanentes représentant 0,8 % du PIB (0,3 milliards de dollars, en dollars courants, augmentant en fonction du PIB par la suite) seraient nécessaires pour stabiliser la dette nette du gouvernement à long terme (en proportion de l’économie).</t>
+  </si>
+  <si>
+    <t>La politique budgétaire actuelle n'est pas viable à long terme. Des hausses d’impôts ou des réductions de dépenses permanentes représentant 0,2 % du PIB (1,8 milliards de dollars, en dollars courants, augmentant en fonction du PIB par la suite) seraient nécessaires pour stabiliser la dette nette du gouvernement à long terme (en proportion de l’économie).</t>
+  </si>
+  <si>
+    <t>Current fiscal policy is not sustainable over the long term. Permanent tax increases or spending reductions amounting to 0.2 per cent of GDP ($1.8 billion in current dollars, growing in line with GDP thereafter) would be required to stabilize government net debt (as a share of the economy) in the long term.</t>
+  </si>
+  <si>
+    <t>Alberta's long-term outlook for population growth is the highest in Canada. In the long run, Alberta is projected to have the fastest growing economy. This is mainly due to favourable demographics resulting in faster growth in total hours worked compared to the national average while labour productivity growth remains on par.</t>
+  </si>
+  <si>
+    <t>British Columbia’s long-term outlook for population growth is in line with the national average. In the long run, British Columbia is projected to have slower real GDP growth compared to the national average. This is mainly due to slower growth in labour productivity compared to the national average.</t>
+  </si>
+  <si>
+    <t>Manitoba's long-term outlook for population growth is in line with the national average. In the long run, Manitoba's real GDP growth is projected to be slightly higher than the national average. This is mainly due to growth in labour productivity catching up to and surpassing the national trend.</t>
+  </si>
+  <si>
+    <t>New Brunswick's long-term outlook for population growth is lower than the national average. In the long run, New Brunswick is projected to have the slowest growing economy. This is due to faster growth among older age groups putting downward pressure on growth in total hours worked and due to lower labour productivity growth compared to the national average.</t>
+  </si>
+  <si>
+    <t>Newfoundland and Labrador's long-term outlook for population growth is the lowest in Canada. In spite of showcasing the highest rates of labour productivity growth in Canada, in the long run, Newfoundland and Labrador is projected to have the slowest real GDP growth compared to the national average. This is due to an ageing population and slow population growth.</t>
+  </si>
+  <si>
+    <t>Nova Scotia's long-term outlook for population growth is lower than the national average. In the long run, Nova Scotia's real GDP growth is projected to be lower than the national average. This mainly due to having one of the lowest growth in total hours worked which in turn is attributable to a relatively older and ageing population.</t>
+  </si>
+  <si>
+    <t>Ontario's long-term outlook for population growth is in line with the national average. In the long run, Ontario is projected to have real GDP growth that is on par with the national average. This is mainly due to labour productivity growing that is slightly faster than the national average.</t>
+  </si>
+  <si>
+    <t>Prince Edward Island's long-term outlook for population growth is slightly below the national average. In the long run, Prince Edward Island is projected to have lower real GDP growth compared to the national average. This is due to slower population growth and population ageing as well as slower growth in labour productivity, though its overall outlook is favourable compared to the other Atlantic provinces.</t>
+  </si>
+  <si>
+    <t>Quebec's long-term outlook for population growth is lower than the national average. In the long run, Quebec's real GDP growth is projected to be lower than the national average. This is mainly due to lower labour productivity growth and stagnant growth in total hours worked.</t>
+  </si>
+  <si>
+    <t>Saskatchewan's long-term outlook for population growth is among the highest in Canada. In the long run, Saskatchewan is projected to have one of the fastest growing economies. This is due to favourable demographic conditions positively impacting growth in total hours worked and higher labour productivity growth compared to the national average.</t>
+  </si>
+  <si>
+    <t>The territories' long-term outlook for population is below the national average, though its population is significantly younger. In the long run, the territories are projected to have slightly lower real GDP growth compared to the national average. Less favourable demographic conditions explain its lower economic growth compared to the national average.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +552,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,6 +571,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -566,12 +590,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -580,14 +601,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -954,235 +977,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7255F49-EEAA-44D0-BDAF-26A02A9AE815}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="66.1328125" customWidth="1"/>
+    <col min="3" max="3" width="68.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="171" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="225" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="3" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="B21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1196,2467 +1219,2479 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59BEA0E-1C9D-4B0B-A62B-B75C30F6159A}">
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J137" sqref="J137"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="6"/>
+    <col min="1" max="1" width="26.86328125" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="3" max="5" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="4">
         <v>2027</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4">
         <v>2052</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="4">
         <v>2077</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>1.2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>0.6</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>32.229999999999997</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>37.42</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>42.71</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1.5</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.5</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>1.2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>3.5</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>3.7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>3.8</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>3.9</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>3.9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>26.9</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>26.4</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>25.6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>25.9</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>1.3</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.4</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1.5</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.9</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>19.2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>13.6</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>13.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>1.3</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>24.94</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>30.92</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>36.17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>3.2</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>2.1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>2.1</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>1.2</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>5.3</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>4.2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>4.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>3.6</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>3.9</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>3.9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>19.2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>18.2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>18.7</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>0.4</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>0.7</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>0</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>2.7</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>-5</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>-4.8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>1.4</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>0.6</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>33.06</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>39.79</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>46.51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>1.9</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>0.9</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>1.2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>16</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>1.2</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>0.3</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>0.8</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>0.7</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>3.9</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>2.9</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>3.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>3.7</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>3.9</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>3.9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>25.2</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>25.5</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>26.2</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>27.1</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>27.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>16</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>-1</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>-1.6</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>2.8</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>16</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="5">
         <v>10.4</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>65.900000000000006</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <v>112.3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>17</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>0.8</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>17</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>38.39</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <v>32.049999999999997</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>28.3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>1.7</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>1.8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>17</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>1.2</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>0.6</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="5">
         <v>1.3</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>1.2</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="5">
         <v>1.2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>17</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>3.7</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>3.8</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>17</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>3.8</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>4</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>17</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>30.9</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>29.3</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>17</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="5">
         <v>30.5</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>31.5</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>17</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="5">
         <v>0.4</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>-4.2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>17</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="5">
         <v>2.6</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>3.7</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>6.8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>17</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="5">
         <v>36.299999999999997</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="5">
         <v>84.6</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="5">
         <v>177.1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>18</v>
       </c>
       <c r="B50" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="5">
         <v>0.5</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <v>0</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
         <v>0.3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>18</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>40.47</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="6">
         <v>44.94</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="6">
         <v>49.01</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>18</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="5">
         <v>1</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="5">
         <v>0.8</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>18</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C53" s="5">
         <v>0.2</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="5">
         <v>-0.1</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>18</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="5">
         <v>1</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="5">
         <v>0.9</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="5">
         <v>3.1</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="5">
         <v>2.8</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="5">
         <v>3.1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>18</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="5">
         <v>3.9</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="5">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>18</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57" s="5">
         <v>32.9</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="5">
         <v>33.6</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="5">
         <v>33.6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>18</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C58" s="5">
         <v>31.1</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="5">
         <v>32.5</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58" s="5">
         <v>32.9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C59" s="5">
         <v>1.8</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>18</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C60" s="5">
         <v>1.9</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D60" s="5">
         <v>0.8</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>18</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="6">
+      <c r="C61" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D61" s="5">
         <v>5.6</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="5">
         <v>-5.4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>14</v>
       </c>
       <c r="B62" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C62" s="5">
         <v>-0.3</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62" s="5">
         <v>-0.7</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="5">
         <v>-0.3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>14</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="3">
         <v>44.04</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D63" s="3">
         <v>54.61</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="3">
         <v>59.06</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>14</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C64" s="5">
         <v>0.6</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="5">
         <v>0.8</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E64" s="5">
         <v>1.2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>14</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="6">
+      <c r="C65" s="5">
         <v>-0.9</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65" s="5">
         <v>-0.7</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E65" s="5">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>14</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C66" s="5">
         <v>1.7</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="5">
         <v>1.6</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E66" s="5">
         <v>1.6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>14</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C67" s="5">
         <v>2.6</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67" s="5">
         <v>2.8</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E67" s="5">
         <v>3.2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>14</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68" s="5">
         <v>3.9</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="5">
         <v>4.2</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E68" s="5">
         <v>4.2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>14</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69" s="5">
         <v>24</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69" s="5">
         <v>23.8</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E69" s="5">
         <v>23.5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>14</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C70" s="5">
         <v>22.2</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="5">
         <v>23.9</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70" s="5">
         <v>24.1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>14</v>
       </c>
       <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C71" s="5">
         <v>1.8</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="5">
         <v>-0.1</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E71" s="5">
         <v>-0.6</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>14</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="6">
+      <c r="C72" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E72" s="5">
         <v>3.4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>14</v>
       </c>
       <c r="B73" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="6">
+      <c r="C73" s="5">
         <v>30.4</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="5">
         <v>43.6</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73" s="5">
         <v>78.8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>19</v>
       </c>
       <c r="B74" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C74" s="5">
         <v>0.7</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="5">
         <v>0</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74" s="5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>19</v>
       </c>
       <c r="B75" t="s">
         <v>3</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="3">
         <v>37.99</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D75" s="3">
         <v>42.74</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="3">
         <v>50.61</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>19</v>
       </c>
       <c r="B76" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="6">
+      <c r="C76" s="5">
         <v>1.4</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76" s="5">
         <v>0.7</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>19</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="6">
+      <c r="C77" s="5">
         <v>0.4</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77" s="5">
         <v>-0.2</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77" s="5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>19</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C78" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78" s="5">
         <v>1</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>19</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C79" s="5">
         <v>3.4</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79" s="5">
         <v>2.7</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="5">
         <v>3.2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>19</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
       </c>
-      <c r="C80" s="6">
+      <c r="C80" s="5">
         <v>4</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80" s="5">
         <v>4</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>19</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
-      <c r="C81" s="6">
+      <c r="C81" s="5">
         <v>32.700000000000003</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81" s="5">
         <v>32.6</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5">
         <v>32.5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>19</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C82" s="5">
         <v>29.6</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="5">
         <v>31.2</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="5">
         <v>31.9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>19</v>
       </c>
       <c r="B83" t="s">
         <v>11</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C83" s="5">
         <v>3.1</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="5">
         <v>1.5</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>19</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="5">
         <v>1.2</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="5">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="5">
         <v>-2.8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>19</v>
       </c>
       <c r="B85" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C85" s="5">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85" s="5">
         <v>-39.299999999999997</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85" s="5">
         <v>-76.8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>20</v>
       </c>
       <c r="B86" t="s">
         <v>2</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="5">
         <v>1.3</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86" s="5">
         <v>0.7</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E86" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>20</v>
       </c>
       <c r="B87" t="s">
         <v>3</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="3">
         <v>31.08</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D87" s="3">
         <v>36.74</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="3">
         <v>43.7</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>20</v>
       </c>
       <c r="B88" t="s">
         <v>4</v>
       </c>
-      <c r="C88" s="6">
+      <c r="C88" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D88" s="5">
         <v>1.6</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E88" s="5">
         <v>1.8</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>20</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="6">
+      <c r="C89" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D89" s="5">
         <v>0.5</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E89" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>20</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="6">
+      <c r="C90" s="5">
         <v>1.2</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>20</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
       </c>
-      <c r="C91" s="6">
+      <c r="C91" s="5">
         <v>4.2</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D91" s="5">
         <v>3.6</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91" s="5">
         <v>3.8</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>20</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
       </c>
-      <c r="C92" s="6">
+      <c r="C92" s="5">
         <v>3.7</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92" s="5">
         <v>3.9</v>
       </c>
-      <c r="E92" s="6">
+      <c r="E92" s="5">
         <v>3.9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>20</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
-      <c r="C93" s="6">
+      <c r="C93" s="5">
         <v>25.8</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D93" s="5">
         <v>25.6</v>
       </c>
-      <c r="E93" s="6">
+      <c r="E93" s="5">
         <v>25.5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>20</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="6">
+      <c r="C94" s="5">
         <v>24.6</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94" s="5">
         <v>25.5</v>
       </c>
-      <c r="E94" s="6">
+      <c r="E94" s="5">
         <v>25.9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>20</v>
       </c>
       <c r="B95" t="s">
         <v>11</v>
       </c>
-      <c r="C95" s="6">
+      <c r="C95" s="5">
         <v>1.2</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D95" s="5">
         <v>0.1</v>
       </c>
-      <c r="E95" s="6">
+      <c r="E95" s="5">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>20</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="6">
+      <c r="C96" s="5">
         <v>1.5</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96" s="5">
         <v>1</v>
       </c>
-      <c r="E96" s="6">
+      <c r="E96" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>20</v>
       </c>
       <c r="B97" t="s">
         <v>13</v>
       </c>
-      <c r="C97" s="6">
+      <c r="C97" s="5">
         <v>26.9</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="5">
         <v>20.399999999999999</v>
       </c>
-      <c r="E97" s="6">
+      <c r="E97" s="5">
         <v>27.2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>21</v>
       </c>
       <c r="B98" t="s">
         <v>2</v>
       </c>
-      <c r="C98" s="6">
+      <c r="C98" s="5">
         <v>1.2</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="5">
         <v>0.6</v>
       </c>
-      <c r="E98" s="6">
+      <c r="E98" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>21</v>
       </c>
       <c r="B99" t="s">
         <v>3</v>
       </c>
-      <c r="C99" s="4">
+      <c r="C99" s="3">
         <v>33.69</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D99" s="3">
         <v>39.53</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E99" s="3">
         <v>50.51</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>21</v>
       </c>
       <c r="B100" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="6">
+      <c r="C100" s="5">
         <v>2.1</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100" s="5">
         <v>1.4</v>
       </c>
-      <c r="E100" s="6">
+      <c r="E100" s="5">
         <v>1.6</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>21</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="6">
+      <c r="C101" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="5">
         <v>0.4</v>
       </c>
-      <c r="E101" s="6">
+      <c r="E101" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>21</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="6">
+      <c r="C102" s="5">
         <v>1.2</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D102" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E102" s="6">
+      <c r="E102" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>21</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="6">
+      <c r="C103" s="5">
         <v>4.2</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D103" s="5">
         <v>3.4</v>
       </c>
-      <c r="E103" s="6">
+      <c r="E103" s="5">
         <v>3.6</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>21</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
       </c>
-      <c r="C104" s="6">
+      <c r="C104" s="5">
         <v>4</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D104" s="5">
         <v>4.2</v>
       </c>
-      <c r="E104" s="6">
+      <c r="E104" s="5">
         <v>4.2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>21</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="6">
+      <c r="C105" s="5">
         <v>34.200000000000003</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D105" s="5">
         <v>33.700000000000003</v>
       </c>
-      <c r="E105" s="6">
+      <c r="E105" s="5">
         <v>33.6</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>21</v>
       </c>
       <c r="B106" t="s">
         <v>10</v>
       </c>
-      <c r="C106" s="6">
+      <c r="C106" s="5">
         <v>33.9</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D106" s="5">
         <v>35.6</v>
       </c>
-      <c r="E106" s="6">
+      <c r="E106" s="5">
         <v>37.1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>21</v>
       </c>
       <c r="B107" t="s">
         <v>11</v>
       </c>
-      <c r="C107" s="6">
+      <c r="C107" s="5">
         <v>0.3</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D107" s="5">
         <v>-1.8</v>
       </c>
-      <c r="E107" s="6">
+      <c r="E107" s="5">
         <v>-3.5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>21</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="6">
+      <c r="C108" s="5">
         <v>1.5</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D108" s="5">
         <v>2.5</v>
       </c>
-      <c r="E108" s="6">
+      <c r="E108" s="5">
         <v>5.5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>21</v>
       </c>
       <c r="B109" t="s">
         <v>13</v>
       </c>
-      <c r="C109" s="6">
+      <c r="C109" s="5">
         <v>22</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D109" s="5">
         <v>58.2</v>
       </c>
-      <c r="E109" s="6">
+      <c r="E109" s="5">
         <v>139.9</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>22</v>
       </c>
       <c r="B110" t="s">
         <v>2</v>
       </c>
-      <c r="C110" s="6">
+      <c r="C110" s="5">
         <v>0.5</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D110" s="5">
         <v>0.2</v>
       </c>
-      <c r="E110" s="6">
+      <c r="E110" s="5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>22</v>
       </c>
       <c r="B111" t="s">
         <v>3</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C111" s="3">
         <v>37.380000000000003</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D111" s="3">
         <v>42.58</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E111" s="3">
         <v>44.03</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>22</v>
       </c>
       <c r="B112" t="s">
         <v>4</v>
       </c>
-      <c r="C112" s="6">
+      <c r="C112" s="5">
         <v>1</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D112" s="5">
         <v>0.9</v>
       </c>
-      <c r="E112" s="6">
+      <c r="E112" s="5">
         <v>1.2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>22</v>
       </c>
       <c r="B113" t="s">
         <v>5</v>
       </c>
-      <c r="C113" s="6">
+      <c r="C113" s="5">
         <v>0.2</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D113" s="5">
         <v>0.1</v>
       </c>
-      <c r="E113" s="6">
+      <c r="E113" s="5">
         <v>0.3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>22</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
       </c>
-      <c r="C114" s="6">
+      <c r="C114" s="5">
         <v>1</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D114" s="5">
         <v>0.9</v>
       </c>
-      <c r="E114" s="6">
+      <c r="E114" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>22</v>
       </c>
       <c r="B115" t="s">
         <v>7</v>
       </c>
-      <c r="C115" s="6">
+      <c r="C115" s="5">
         <v>3.1</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D115" s="5">
         <v>2.9</v>
       </c>
-      <c r="E115" s="6">
+      <c r="E115" s="5">
         <v>3.2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>22</v>
       </c>
       <c r="B116" t="s">
         <v>8</v>
       </c>
-      <c r="C116" s="6">
+      <c r="C116" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D116" s="5">
         <v>4</v>
       </c>
-      <c r="E116" s="6">
+      <c r="E116" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>22</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
       </c>
-      <c r="C117" s="6">
+      <c r="C117" s="5">
         <v>34.5</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D117" s="5">
         <v>35.5</v>
       </c>
-      <c r="E117" s="6">
+      <c r="E117" s="5">
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>22</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
       </c>
-      <c r="C118" s="6">
+      <c r="C118" s="5">
         <v>31.4</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D118" s="5">
         <v>32.5</v>
       </c>
-      <c r="E118" s="6">
+      <c r="E118" s="5">
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>22</v>
       </c>
       <c r="B119" t="s">
         <v>11</v>
       </c>
-      <c r="C119" s="6">
+      <c r="C119" s="5">
         <v>3.2</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D119" s="5">
         <v>2.9</v>
       </c>
-      <c r="E119" s="6">
+      <c r="E119" s="5">
         <v>2.5</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>22</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
       </c>
-      <c r="C120" s="6">
+      <c r="C120" s="5">
         <v>2.5</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D120" s="5">
         <v>-0.1</v>
       </c>
-      <c r="E120" s="6">
+      <c r="E120" s="5">
         <v>-2.9</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>22</v>
       </c>
       <c r="B121" t="s">
         <v>13</v>
       </c>
-      <c r="C121" s="6">
+      <c r="C121" s="5">
         <v>25.7</v>
       </c>
-      <c r="D121" s="6">
+      <c r="D121" s="5">
         <v>-21.6</v>
       </c>
-      <c r="E121" s="6">
+      <c r="E121" s="5">
         <v>-87</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>23</v>
       </c>
       <c r="B122" t="s">
         <v>2</v>
       </c>
-      <c r="C122" s="6">
+      <c r="C122" s="5">
         <v>1.3</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D122" s="5">
         <v>0.9</v>
       </c>
-      <c r="E122" s="6">
+      <c r="E122" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>23</v>
       </c>
       <c r="B123" t="s">
         <v>3</v>
       </c>
-      <c r="C123" s="4">
+      <c r="C123" s="3">
         <v>29.25</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D123" s="3">
         <v>32.31</v>
       </c>
-      <c r="E123" s="4">
+      <c r="E123" s="3">
         <v>38.17</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>23</v>
       </c>
       <c r="B124" t="s">
         <v>4</v>
       </c>
-      <c r="C124" s="6">
+      <c r="C124" s="5">
         <v>2.7</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D124" s="5">
         <v>2</v>
       </c>
-      <c r="E124" s="6">
+      <c r="E124" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>23</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
       </c>
-      <c r="C125" s="6">
+      <c r="C125" s="5">
         <v>1.4</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D125" s="5">
         <v>0.7</v>
       </c>
-      <c r="E125" s="6">
+      <c r="E125" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>23</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
       </c>
-      <c r="C126" s="6">
+      <c r="C126" s="5">
         <v>1.4</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D126" s="5">
         <v>1.3</v>
       </c>
-      <c r="E126" s="6">
+      <c r="E126" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>23</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
       </c>
-      <c r="C127" s="6">
+      <c r="C127" s="5">
         <v>4.7</v>
       </c>
-      <c r="D127" s="6">
+      <c r="D127" s="5">
         <v>4</v>
       </c>
-      <c r="E127" s="6">
+      <c r="E127" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>23</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
       </c>
-      <c r="C128" s="6">
+      <c r="C128" s="5">
         <v>3.6</v>
       </c>
-      <c r="D128" s="6">
+      <c r="D128" s="5">
         <v>3.9</v>
       </c>
-      <c r="E128" s="6">
+      <c r="E128" s="5">
         <v>3.9</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>23</v>
       </c>
       <c r="B129" t="s">
         <v>9</v>
       </c>
-      <c r="C129" s="6">
+      <c r="C129" s="5">
         <v>26.1</v>
       </c>
-      <c r="D129" s="6">
+      <c r="D129" s="5">
         <v>25.8</v>
       </c>
-      <c r="E129" s="6">
+      <c r="E129" s="5">
         <v>25.6</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>23</v>
       </c>
       <c r="B130" t="s">
         <v>10</v>
       </c>
-      <c r="C130" s="6">
+      <c r="C130" s="5">
         <v>23.4</v>
       </c>
-      <c r="D130" s="6">
+      <c r="D130" s="5">
         <v>23.8</v>
       </c>
-      <c r="E130" s="6">
+      <c r="E130" s="5">
         <v>24.1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>23</v>
       </c>
       <c r="B131" t="s">
         <v>11</v>
       </c>
-      <c r="C131" s="6">
+      <c r="C131" s="5">
         <v>2.6</v>
       </c>
-      <c r="D131" s="6">
+      <c r="D131" s="5">
         <v>2</v>
       </c>
-      <c r="E131" s="6">
+      <c r="E131" s="5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>23</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
       </c>
-      <c r="C132" s="6">
+      <c r="C132" s="5">
         <v>0.9</v>
       </c>
-      <c r="D132" s="6">
+      <c r="D132" s="5">
         <v>-1.2</v>
       </c>
-      <c r="E132" s="6">
+      <c r="E132" s="5">
         <v>-2.8</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>23</v>
       </c>
       <c r="B133" t="s">
         <v>13</v>
       </c>
-      <c r="C133" s="6">
+      <c r="C133" s="5">
         <v>-0.2</v>
       </c>
-      <c r="D133" s="6">
+      <c r="D133" s="5">
         <v>-42</v>
       </c>
-      <c r="E133" s="6">
+      <c r="E133" s="5">
         <v>-79.099999999999994</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>24</v>
       </c>
       <c r="B134" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="6">
+      <c r="C134" s="5">
         <v>0.9</v>
       </c>
-      <c r="D134" s="6">
+      <c r="D134" s="5">
         <v>0.4</v>
       </c>
-      <c r="E134" s="6">
+      <c r="E134" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>24</v>
       </c>
       <c r="B135" t="s">
         <v>3</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C135" s="3">
         <v>17.41</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D135" s="3">
         <v>23.62</v>
       </c>
-      <c r="E135" s="4">
+      <c r="E135" s="3">
         <v>25.51</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>24</v>
       </c>
       <c r="B136" t="s">
         <v>4</v>
       </c>
-      <c r="C136" s="6">
+      <c r="C136" s="5">
         <v>2</v>
       </c>
-      <c r="D136" s="6">
+      <c r="D136" s="5">
         <v>1.2</v>
       </c>
-      <c r="E136" s="6">
+      <c r="E136" s="5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>24</v>
       </c>
       <c r="B137" t="s">
         <v>5</v>
       </c>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C137" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="D137" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="E137" s="7">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>24</v>
       </c>
       <c r="B138" t="s">
         <v>6</v>
       </c>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C138" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="D138" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E138" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>24</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
       </c>
-      <c r="C139" s="6">
+      <c r="C139" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D139" s="6">
+      <c r="D139" s="5">
         <v>3.3</v>
       </c>
-      <c r="E139" s="6">
+      <c r="E139" s="5">
         <v>3.5</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>24</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
       </c>
-      <c r="C140" s="6">
+      <c r="C140" s="5">
         <v>4</v>
       </c>
-      <c r="D140" s="6">
+      <c r="D140" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E140" s="6">
+      <c r="E140" s="5">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>24</v>
       </c>
       <c r="B141" t="s">
         <v>9</v>
       </c>
-      <c r="C141" s="6">
+      <c r="C141" s="5">
         <v>53.2</v>
       </c>
-      <c r="D141" s="6">
+      <c r="D141" s="5">
         <v>53.7</v>
       </c>
-      <c r="E141" s="6">
+      <c r="E141" s="5">
         <v>53.7</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>24</v>
       </c>
       <c r="B142" t="s">
         <v>10</v>
       </c>
-      <c r="C142" s="6">
+      <c r="C142" s="5">
         <v>57.8</v>
       </c>
-      <c r="D142" s="6">
+      <c r="D142" s="5">
         <v>59.6</v>
       </c>
-      <c r="E142" s="6">
+      <c r="E142" s="5">
         <v>60.3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>24</v>
       </c>
       <c r="B143" t="s">
         <v>11</v>
       </c>
-      <c r="C143" s="6">
+      <c r="C143" s="5">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="D143" s="6">
+      <c r="D143" s="5">
         <v>-5.9</v>
       </c>
-      <c r="E143" s="6">
+      <c r="E143" s="5">
         <v>-6.6</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>24</v>
       </c>
       <c r="B144" t="s">
         <v>12</v>
       </c>
-      <c r="C144" s="6">
+      <c r="C144" s="5">
         <v>1.2</v>
       </c>
-      <c r="D144" s="6">
+      <c r="D144" s="5">
         <v>7.7</v>
       </c>
-      <c r="E144" s="6">
+      <c r="E144" s="5">
         <v>15.7</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>24</v>
       </c>
       <c r="B145" t="s">
         <v>13</v>
       </c>
-      <c r="C145" s="6">
+      <c r="C145" s="5">
         <v>15.1</v>
       </c>
-      <c r="D145" s="6">
+      <c r="D145" s="5">
         <v>194.9</v>
       </c>
-      <c r="E145" s="6">
+      <c r="E145" s="5">
         <v>406.2</v>
       </c>
     </row>
@@ -3675,14 +3710,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1"/>
+    <col min="4" max="4" width="21.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -3690,13 +3725,13 @@
         <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3704,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -3712,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3720,7 +3755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3728,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3736,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3744,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3752,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -3760,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3768,7 +3803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3776,7 +3811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -3795,330 +3830,325 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C496FAE6-5834-4DFC-B56D-04D2AE526F4F}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="2" max="2" width="64.3984375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="64.265625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="131.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>46</v>
+      <c r="B34" s="12" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4136,17 +4166,17 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -4392,7 +4422,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4643,7 +4673,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4894,7 +4924,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -5145,7 +5175,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5396,7 +5426,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5647,7 +5677,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -5898,7 +5928,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -6149,7 +6179,7 @@
         <v>242.4</v>
       </c>
     </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -6400,7 +6430,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -6651,7 +6681,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -6902,7 +6932,7 @@
         <v>-9.9</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -7153,7 +7183,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -7404,7 +7434,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -7655,7 +7685,7 @@
         <v>102.4</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -7906,7 +7936,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -8157,7 +8187,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -8408,7 +8438,7 @@
         <v>-85.4</v>
       </c>
     </row>
-    <row r="18" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -8659,7 +8689,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -8910,7 +8940,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -9161,7 +9191,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -9412,7 +9442,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="22" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -9663,7 +9693,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -9914,7 +9944,7 @@
         <v>204.9</v>
       </c>
     </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -10165,7 +10195,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -10416,7 +10446,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="26" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -10667,7 +10697,7 @@
         <v>-125.1</v>
       </c>
     </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -10918,7 +10948,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -11169,7 +11199,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="29" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -11420,7 +11450,7 @@
         <v>-94.5</v>
       </c>
     </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -11671,7 +11701,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -11922,7 +11952,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -12173,7 +12203,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="33" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -12424,7 +12454,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="34" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:83" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>24</v>
       </c>

</xml_diff>